<commit_message>
einde laptop, overgang naar pc
</commit_message>
<xml_diff>
--- a/xls/preparingtables.xlsx
+++ b/xls/preparingtables.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="20730" windowHeight="6435" tabRatio="823" firstSheet="4" activeTab="10"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="20730" windowHeight="6435" tabRatio="892" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="struct_sf16_eng" sheetId="8" r:id="rId1"/>
     <sheet name="struct_sf16_nld" sheetId="31" r:id="rId2"/>
     <sheet name="outline_sf16_eng" sheetId="17" r:id="rId3"/>
-    <sheet name="levelmax_sf16_995" sheetId="9" r:id="rId4"/>
-    <sheet name="levelmax_sf16_993" sheetId="22" r:id="rId5"/>
-    <sheet name="ex1_data" sheetId="19" r:id="rId6"/>
-    <sheet name="ex2_data" sheetId="20" r:id="rId7"/>
-    <sheet name="ex3_struct" sheetId="25" r:id="rId8"/>
-    <sheet name="ex3_struct_test" sheetId="27" r:id="rId9"/>
+    <sheet name="outline_sf16_nld" sheetId="32" r:id="rId4"/>
+    <sheet name="levelmax_sf16_995" sheetId="9" r:id="rId5"/>
+    <sheet name="levelmax_sf16_993" sheetId="22" r:id="rId6"/>
+    <sheet name="ex1_data" sheetId="19" r:id="rId7"/>
+    <sheet name="ex2_data" sheetId="20" r:id="rId8"/>
+    <sheet name="ex3_struct" sheetId="25" r:id="rId9"/>
     <sheet name="ex3_data" sheetId="24" r:id="rId10"/>
-    <sheet name="outline_exceptions" sheetId="23" r:id="rId11"/>
+    <sheet name="ex4_outline" sheetId="23" r:id="rId11"/>
     <sheet name="ex3_data_test" sheetId="28" r:id="rId12"/>
     <sheet name="ex3_data (2)" sheetId="30" r:id="rId13"/>
     <sheet name="ex3_levelmax" sheetId="26" r:id="rId14"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="117">
   <si>
     <t>2d</t>
   </si>
@@ -1490,9 +1490,7 @@
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2901,7 +2899,7 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3809,88 +3807,228 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor theme="6" tint="-0.249977111117893"/>
+    <tabColor theme="6" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>35</v>
       </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>36</v>
       </c>
-      <c r="B9">
-        <v>5</v>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3942,7 +4080,7 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3950,7 +4088,7 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3958,7 +4096,7 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -3966,7 +4104,7 @@
         <v>35</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3974,7 +4112,7 @@
         <v>36</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -3983,6 +4121,94 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="6" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
@@ -4186,7 +4412,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT3"/>
   <sheetViews>
@@ -4676,7 +4902,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -4807,405 +5033,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="6" tint="-0.249977111117893"/>
-  </sheetPr>
-  <dimension ref="A1:E43"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="18">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="19">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="2">
-        <v>3</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="2">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="2">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" s="4">
-        <v>3</v>
-      </c>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="4"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="4"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>64</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>57</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C36" s="4"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>58</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>59</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>60</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>61</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>62</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C43" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
steps taken in documentation
</commit_message>
<xml_diff>
--- a/xls/preparingtables.xlsx
+++ b/xls/preparingtables.xlsx
@@ -4,31 +4,28 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="6420" windowWidth="28800" windowHeight="6480" tabRatio="904"/>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="28800" windowHeight="6435" tabRatio="823" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="-15" yWindow="6420" windowWidth="28800" windowHeight="6480" tabRatio="904" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="struct_sf16_eng" sheetId="8" r:id="rId1"/>
-    <sheet name="outline_sf16_eng" sheetId="17" r:id="rId2"/>
-    <sheet name="outline_sf16_eng_exceptions" sheetId="23" r:id="rId3"/>
-    <sheet name="levelmax_sf16_995" sheetId="9" r:id="rId4"/>
-    <sheet name="levelmax_sf16_993" sheetId="22" r:id="rId5"/>
-    <sheet name="example1_sf16_eng" sheetId="19" r:id="rId6"/>
-    <sheet name="example2_sf16_eng" sheetId="20" r:id="rId7"/>
-    <sheet name="ex3_struct" sheetId="25" r:id="rId8"/>
-    <sheet name="ex3_struct_test" sheetId="27" r:id="rId9"/>
+    <sheet name="struct_sf16_nld" sheetId="31" r:id="rId2"/>
+    <sheet name="outline_sf16_eng" sheetId="17" r:id="rId3"/>
+    <sheet name="outline_sf16_nld" sheetId="32" r:id="rId4"/>
+    <sheet name="levelmax_sf16_995" sheetId="9" r:id="rId5"/>
+    <sheet name="levelmax_sf16_993" sheetId="22" r:id="rId6"/>
+    <sheet name="ex1_data" sheetId="19" r:id="rId7"/>
+    <sheet name="ex2_data" sheetId="20" r:id="rId8"/>
+    <sheet name="ex3_struct" sheetId="25" r:id="rId9"/>
     <sheet name="ex3_data" sheetId="24" r:id="rId10"/>
-    <sheet name="ex3_data_test" sheetId="28" r:id="rId11"/>
-    <sheet name="ex3_data (2)" sheetId="30" r:id="rId12"/>
-    <sheet name="ex3_levelmax" sheetId="26" r:id="rId13"/>
-    <sheet name="ex3_levelmax_test" sheetId="29" r:id="rId14"/>
+    <sheet name="ex3_levelmax" sheetId="26" r:id="rId11"/>
+    <sheet name="ex4_outline" sheetId="23" r:id="rId12"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="117">
   <si>
     <t>2d</t>
   </si>
@@ -259,6 +256,126 @@
   </si>
   <si>
     <t>m_illiquidity</t>
+  </si>
+  <si>
+    <t>SKV</t>
+  </si>
+  <si>
+    <t>KernSKV</t>
+  </si>
+  <si>
+    <t>operationeel</t>
+  </si>
+  <si>
+    <t>LACDT</t>
+  </si>
+  <si>
+    <t>KSKV-div</t>
+  </si>
+  <si>
+    <t>markt</t>
+  </si>
+  <si>
+    <t>leven</t>
+  </si>
+  <si>
+    <t>schade</t>
+  </si>
+  <si>
+    <t>tegenpartijkrediet</t>
+  </si>
+  <si>
+    <t>markt-div</t>
+  </si>
+  <si>
+    <t>m_rente</t>
+  </si>
+  <si>
+    <t>m_aandelen</t>
+  </si>
+  <si>
+    <t>m_vastgoed</t>
+  </si>
+  <si>
+    <t>m_valuta</t>
+  </si>
+  <si>
+    <t>m_concentratie</t>
+  </si>
+  <si>
+    <t>m_illiquiditeit</t>
+  </si>
+  <si>
+    <t>leven-div</t>
+  </si>
+  <si>
+    <t>l_kortleven</t>
+  </si>
+  <si>
+    <t>l_langleven</t>
+  </si>
+  <si>
+    <t>l_ao</t>
+  </si>
+  <si>
+    <t>l_verval</t>
+  </si>
+  <si>
+    <t>l_kosten</t>
+  </si>
+  <si>
+    <t>l_revisie</t>
+  </si>
+  <si>
+    <t>schade-div</t>
+  </si>
+  <si>
+    <t>s_premiereserve</t>
+  </si>
+  <si>
+    <t>s_verval</t>
+  </si>
+  <si>
+    <t>s_CAT</t>
+  </si>
+  <si>
+    <t>zorg-div</t>
+  </si>
+  <si>
+    <t>zorg</t>
+  </si>
+  <si>
+    <t>z_alsleven</t>
+  </si>
+  <si>
+    <t>z_CAT</t>
+  </si>
+  <si>
+    <t>z_s_premiereserve</t>
+  </si>
+  <si>
+    <t>z_s_verval</t>
+  </si>
+  <si>
+    <t>z_alsleven-div</t>
+  </si>
+  <si>
+    <t>z_a_kortleven</t>
+  </si>
+  <si>
+    <t>z_a_langleven</t>
+  </si>
+  <si>
+    <t>z_a_ao</t>
+  </si>
+  <si>
+    <t>z_a_verval</t>
+  </si>
+  <si>
+    <t>z_a_kosten</t>
+  </si>
+  <si>
+    <t>z_a_revisie</t>
   </si>
 </sst>
 </file>
@@ -685,10 +802,9 @@
   </sheetPr>
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1369,15 +1485,12 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor rgb="FFFF0000"/>
+    <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
-    </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="1">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1566,164 +1679,47 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <sheetPr>
+    <tabColor theme="0" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.5703125" style="10" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="17">
-        <v>2</v>
-      </c>
-      <c r="B2" s="17">
-        <v>1</v>
-      </c>
-      <c r="C2" s="17">
-        <v>2015</v>
-      </c>
-      <c r="D2" s="17">
-        <v>230</v>
-      </c>
-      <c r="E2" s="16">
-        <v>91.8</v>
-      </c>
-      <c r="F2" s="17">
-        <v>113</v>
-      </c>
-      <c r="G2" s="17">
-        <v>7</v>
-      </c>
-      <c r="H2" s="16">
-        <v>-30.5</v>
-      </c>
-      <c r="I2" s="17">
-        <v>-31.4</v>
-      </c>
-      <c r="J2" s="17">
-        <v>64.2</v>
-      </c>
-      <c r="K2" s="16">
-        <v>80.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="17">
-        <v>1</v>
-      </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17">
-        <v>2016</v>
-      </c>
-      <c r="D3" s="17">
-        <v>235</v>
-      </c>
-      <c r="E3" s="16">
-        <v>85</v>
-      </c>
-      <c r="F3" s="17">
-        <v>104.62962962962963</v>
-      </c>
-      <c r="G3" s="17">
-        <v>6.4814814814814818</v>
-      </c>
-      <c r="H3" s="16">
-        <v>-28.24074074074074</v>
-      </c>
-      <c r="I3" s="17">
-        <v>-29.074074074074073</v>
-      </c>
-      <c r="J3" s="17">
-        <v>59.44444444444445</v>
-      </c>
-      <c r="K3" s="16">
-        <v>74.259259259259267</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
-        <v>3</v>
-      </c>
-      <c r="B4" s="17">
-        <v>2</v>
-      </c>
-      <c r="C4" s="17">
-        <v>2017</v>
-      </c>
-      <c r="D4" s="17">
-        <v>234</v>
-      </c>
-      <c r="E4" s="16">
-        <v>78.703703703703709</v>
-      </c>
-      <c r="F4" s="17">
-        <v>96.879286694101509</v>
-      </c>
-      <c r="G4" s="17">
-        <v>6.0013717421124833</v>
-      </c>
-      <c r="H4" s="16">
-        <v>-26.14883401920439</v>
-      </c>
-      <c r="I4" s="17">
-        <v>-26.920438957475994</v>
-      </c>
-      <c r="J4" s="17">
-        <v>55.041152263374492</v>
-      </c>
-      <c r="K4" s="16">
-        <v>68.758573388203018</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1733,816 +1729,14 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT4"/>
+  <sheetPr>
+    <tabColor theme="0" tint="-0.34998626667073579"/>
+  </sheetPr>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="R38" sqref="R38"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4" style="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4" style="10" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="4.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="31" max="33" width="4" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="4" style="10" bestFit="1" customWidth="1"/>
-    <col min="35" max="38" width="4" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="4" style="10" bestFit="1" customWidth="1"/>
-    <col min="40" max="46" width="4" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:46" ht="75.75" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="9" t="str">
-        <f t="array" ref="E1:AT1">TRANSPOSE(struct_sf16_eng!A2:A44)</f>
-        <v>SCR</v>
-      </c>
-      <c r="F1" s="11" t="str">
-        <v>BSCR</v>
-      </c>
-      <c r="G1" s="8" t="str">
-        <v>operational</v>
-      </c>
-      <c r="H1" s="9" t="str">
-        <v>Adjustment-LACDT</v>
-      </c>
-      <c r="I1" s="8" t="str">
-        <v>BSCR_div</v>
-      </c>
-      <c r="J1" s="8" t="str">
-        <v>market</v>
-      </c>
-      <c r="K1" s="8" t="str">
-        <v>life</v>
-      </c>
-      <c r="L1" s="8" t="str">
-        <v>nonlife</v>
-      </c>
-      <c r="M1" s="8" t="str">
-        <v>health</v>
-      </c>
-      <c r="N1" s="8" t="str">
-        <v>cp-default</v>
-      </c>
-      <c r="O1" s="9" t="str">
-        <v>intangibles</v>
-      </c>
-      <c r="P1" s="8" t="str">
-        <v>market_div</v>
-      </c>
-      <c r="Q1" s="8" t="str">
-        <v>m_interestrate</v>
-      </c>
-      <c r="R1" s="8" t="str">
-        <v>m_equity</v>
-      </c>
-      <c r="S1" s="8" t="str">
-        <v>m_property</v>
-      </c>
-      <c r="T1" s="8" t="str">
-        <v>m_spread</v>
-      </c>
-      <c r="U1" s="8" t="str">
-        <v>m_currency</v>
-      </c>
-      <c r="V1" s="9" t="str">
-        <v>m_concentration</v>
-      </c>
-      <c r="W1" s="8" t="str">
-        <v>m_illiquidity</v>
-      </c>
-      <c r="X1" s="8" t="str">
-        <v>life_div</v>
-      </c>
-      <c r="Y1" s="8" t="str">
-        <v>l_mortality</v>
-      </c>
-      <c r="Z1" s="8" t="str">
-        <v>l_longevity</v>
-      </c>
-      <c r="AA1" s="8" t="str">
-        <v>l_disability</v>
-      </c>
-      <c r="AB1" s="8" t="str">
-        <v>l_lapse</v>
-      </c>
-      <c r="AC1" s="8" t="str">
-        <v>l_expenses</v>
-      </c>
-      <c r="AD1" s="9" t="str">
-        <v>l_revision</v>
-      </c>
-      <c r="AE1" s="8" t="str">
-        <v>l_CAT</v>
-      </c>
-      <c r="AF1" s="8" t="str">
-        <v>nonlife_div</v>
-      </c>
-      <c r="AG1" s="8" t="str">
-        <v>n_premiumreserve</v>
-      </c>
-      <c r="AH1" s="9" t="str">
-        <v>n_lapse</v>
-      </c>
-      <c r="AI1" s="8" t="str">
-        <v>n_CAT</v>
-      </c>
-      <c r="AJ1" s="8" t="str">
-        <v>health_div</v>
-      </c>
-      <c r="AK1" s="8" t="str">
-        <v>h_SLT</v>
-      </c>
-      <c r="AL1" s="8" t="str">
-        <v>h_CAT</v>
-      </c>
-      <c r="AM1" s="9" t="str">
-        <v>h_n_premiumres</v>
-      </c>
-      <c r="AN1" s="8" t="str">
-        <v>h_n_lapse</v>
-      </c>
-      <c r="AO1" s="8" t="str">
-        <v>h_SLT_div</v>
-      </c>
-      <c r="AP1" s="8" t="str">
-        <v>h_s_mortality</v>
-      </c>
-      <c r="AQ1" s="8" t="str">
-        <v>h_s_longevity</v>
-      </c>
-      <c r="AR1" s="8" t="str">
-        <v>h_s_disability</v>
-      </c>
-      <c r="AS1" s="8" t="str">
-        <v>h_s_lapse</v>
-      </c>
-      <c r="AT1" s="8" t="str">
-        <v>h_s_expenses</v>
-      </c>
-    </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A2" s="17">
-        <v>2</v>
-      </c>
-      <c r="B2" s="17">
-        <v>1</v>
-      </c>
-      <c r="C2" s="17">
-        <v>2015</v>
-      </c>
-      <c r="D2" s="17">
-        <v>230</v>
-      </c>
-      <c r="E2" s="16">
-        <v>91.8</v>
-      </c>
-      <c r="F2" s="17">
-        <v>113</v>
-      </c>
-      <c r="G2" s="17">
-        <v>7</v>
-      </c>
-      <c r="H2" s="16">
-        <v>-30.5</v>
-      </c>
-      <c r="I2" s="17">
-        <v>-31.4</v>
-      </c>
-      <c r="J2" s="17">
-        <v>64.2</v>
-      </c>
-      <c r="K2" s="17">
-        <v>80.2</v>
-      </c>
-      <c r="L2" s="17">
-        <v>0</v>
-      </c>
-      <c r="M2" s="17">
-        <v>0</v>
-      </c>
-      <c r="N2" s="17">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="O2" s="16">
-        <v>0</v>
-      </c>
-      <c r="P2" s="17">
-        <v>-4.7</v>
-      </c>
-      <c r="Q2" s="17">
-        <v>2.7</v>
-      </c>
-      <c r="R2" s="17">
-        <v>10.5</v>
-      </c>
-      <c r="S2" s="17">
-        <v>1.6</v>
-      </c>
-      <c r="T2" s="17">
-        <v>53.5</v>
-      </c>
-      <c r="U2" s="17">
-        <v>0.6</v>
-      </c>
-      <c r="V2" s="16">
-        <v>0</v>
-      </c>
-      <c r="W2" s="17">
-        <v>-44</v>
-      </c>
-      <c r="X2" s="17">
-        <v>29</v>
-      </c>
-      <c r="Y2" s="17">
-        <v>6.1</v>
-      </c>
-      <c r="Z2" s="17">
-        <v>0.4</v>
-      </c>
-      <c r="AA2" s="17">
-        <v>48</v>
-      </c>
-      <c r="AB2" s="17">
-        <v>21.1</v>
-      </c>
-      <c r="AC2" s="17">
-        <v>0</v>
-      </c>
-      <c r="AD2" s="16">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="AE2" s="17">
-        <v>0</v>
-      </c>
-      <c r="AF2" s="17">
-        <v>0</v>
-      </c>
-      <c r="AG2" s="17">
-        <v>0</v>
-      </c>
-      <c r="AH2" s="16">
-        <v>0</v>
-      </c>
-      <c r="AI2" s="17">
-        <v>0</v>
-      </c>
-      <c r="AJ2" s="17">
-        <v>0</v>
-      </c>
-      <c r="AK2" s="17">
-        <v>0</v>
-      </c>
-      <c r="AL2" s="17">
-        <v>0</v>
-      </c>
-      <c r="AM2" s="16">
-        <v>0</v>
-      </c>
-      <c r="AN2" s="17">
-        <v>0</v>
-      </c>
-      <c r="AO2" s="17">
-        <v>0</v>
-      </c>
-      <c r="AP2" s="17">
-        <v>0</v>
-      </c>
-      <c r="AQ2" s="17">
-        <v>0</v>
-      </c>
-      <c r="AR2" s="17">
-        <v>0</v>
-      </c>
-      <c r="AS2" s="17">
-        <v>0</v>
-      </c>
-      <c r="AT2" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A3" s="17">
-        <v>1</v>
-      </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17">
-        <v>2016</v>
-      </c>
-      <c r="D3" s="17">
-        <v>235</v>
-      </c>
-      <c r="E3" s="16">
-        <f>85/$E$2*E2</f>
-        <v>85</v>
-      </c>
-      <c r="F3" s="17">
-        <f t="shared" ref="F3:AD4" si="0">85/$E$2*F2</f>
-        <v>104.62962962962963</v>
-      </c>
-      <c r="G3" s="17">
-        <f t="shared" si="0"/>
-        <v>6.4814814814814818</v>
-      </c>
-      <c r="H3" s="16">
-        <f t="shared" si="0"/>
-        <v>-28.24074074074074</v>
-      </c>
-      <c r="I3" s="17">
-        <f t="shared" si="0"/>
-        <v>-29.074074074074073</v>
-      </c>
-      <c r="J3" s="17">
-        <f t="shared" si="0"/>
-        <v>59.44444444444445</v>
-      </c>
-      <c r="K3" s="17">
-        <f t="shared" si="0"/>
-        <v>74.259259259259267</v>
-      </c>
-      <c r="L3" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M3" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N3" s="17">
-        <f t="shared" si="0"/>
-        <v>2.1296296296296293</v>
-      </c>
-      <c r="O3" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P3" s="17">
-        <f t="shared" si="0"/>
-        <v>-4.3518518518518521</v>
-      </c>
-      <c r="Q3" s="17">
-        <f>85/$E$2*Q2+3</f>
-        <v>5.5</v>
-      </c>
-      <c r="R3" s="17">
-        <f>85/$E$2*R2+5</f>
-        <v>14.722222222222221</v>
-      </c>
-      <c r="S3" s="17">
-        <f>85/$E$2*S2+2</f>
-        <v>3.4814814814814818</v>
-      </c>
-      <c r="T3" s="17">
-        <f>85/$E$2*T2-10</f>
-        <v>39.537037037037038</v>
-      </c>
-      <c r="U3" s="17">
-        <f t="shared" si="0"/>
-        <v>0.55555555555555558</v>
-      </c>
-      <c r="V3" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W3" s="17">
-        <f t="shared" si="0"/>
-        <v>-40.74074074074074</v>
-      </c>
-      <c r="X3" s="17">
-        <f>85/$E$2*X2-3</f>
-        <v>23.851851851851851</v>
-      </c>
-      <c r="Y3" s="17">
-        <f>85/$E$2*Y2-1</f>
-        <v>4.6481481481481479</v>
-      </c>
-      <c r="Z3" s="17">
-        <f t="shared" si="0"/>
-        <v>0.37037037037037041</v>
-      </c>
-      <c r="AA3" s="17">
-        <f>85/$E$2*AA2+4</f>
-        <v>48.444444444444443</v>
-      </c>
-      <c r="AB3" s="17">
-        <f t="shared" si="0"/>
-        <v>19.537037037037038</v>
-      </c>
-      <c r="AC3" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AD3" s="16">
-        <f t="shared" si="0"/>
-        <v>18.148148148148149</v>
-      </c>
-      <c r="AE3" s="17">
-        <v>0</v>
-      </c>
-      <c r="AF3" s="17">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="17">
-        <v>0</v>
-      </c>
-      <c r="AH3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="17">
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="17">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="17">
-        <v>0</v>
-      </c>
-      <c r="AL3" s="17">
-        <v>0</v>
-      </c>
-      <c r="AM3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AN3" s="17">
-        <v>0</v>
-      </c>
-      <c r="AO3" s="17">
-        <v>0</v>
-      </c>
-      <c r="AP3" s="17">
-        <v>0</v>
-      </c>
-      <c r="AQ3" s="17">
-        <v>0</v>
-      </c>
-      <c r="AR3" s="17">
-        <v>0</v>
-      </c>
-      <c r="AS3" s="17">
-        <v>0</v>
-      </c>
-      <c r="AT3" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
-        <v>3</v>
-      </c>
-      <c r="B4" s="17">
-        <v>2</v>
-      </c>
-      <c r="C4" s="17">
-        <v>2017</v>
-      </c>
-      <c r="D4" s="17">
-        <v>234</v>
-      </c>
-      <c r="E4" s="16">
-        <f>85/$E$2*E3</f>
-        <v>78.703703703703709</v>
-      </c>
-      <c r="F4" s="17">
-        <f t="shared" si="0"/>
-        <v>96.879286694101509</v>
-      </c>
-      <c r="G4" s="17">
-        <f t="shared" si="0"/>
-        <v>6.0013717421124833</v>
-      </c>
-      <c r="H4" s="16">
-        <f t="shared" si="0"/>
-        <v>-26.14883401920439</v>
-      </c>
-      <c r="I4" s="17">
-        <f t="shared" si="0"/>
-        <v>-26.920438957475994</v>
-      </c>
-      <c r="J4" s="17">
-        <f t="shared" si="0"/>
-        <v>55.041152263374492</v>
-      </c>
-      <c r="K4" s="17">
-        <f t="shared" si="0"/>
-        <v>68.758573388203018</v>
-      </c>
-      <c r="L4" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M4" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N4" s="17">
-        <f t="shared" si="0"/>
-        <v>1.9718792866941013</v>
-      </c>
-      <c r="O4" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P4" s="17">
-        <f t="shared" si="0"/>
-        <v>-4.0294924554183815</v>
-      </c>
-      <c r="Q4" s="17">
-        <f>85/$E$2*Q3+3</f>
-        <v>8.0925925925925917</v>
-      </c>
-      <c r="R4" s="17">
-        <f>85/$E$2*R3+5</f>
-        <v>18.631687242798353</v>
-      </c>
-      <c r="S4" s="17">
-        <f>85/$E$2*S3+2</f>
-        <v>5.2235939643347056</v>
-      </c>
-      <c r="T4" s="17">
-        <f>85/$E$2*T3-10</f>
-        <v>26.60836762688615</v>
-      </c>
-      <c r="U4" s="17">
-        <f t="shared" si="0"/>
-        <v>0.51440329218106995</v>
-      </c>
-      <c r="V4" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W4" s="17">
-        <f t="shared" si="0"/>
-        <v>-37.722908093278463</v>
-      </c>
-      <c r="X4" s="17">
-        <f>85/$E$2*X3-3</f>
-        <v>19.085048010973935</v>
-      </c>
-      <c r="Y4" s="17">
-        <f>85/$E$2*Y3-1</f>
-        <v>3.3038408779149515</v>
-      </c>
-      <c r="Z4" s="17">
-        <f t="shared" si="0"/>
-        <v>0.34293552812071332</v>
-      </c>
-      <c r="AA4" s="17">
-        <f>85/$E$2*AA3+4</f>
-        <v>48.855967078189302</v>
-      </c>
-      <c r="AB4" s="17">
-        <f t="shared" si="0"/>
-        <v>18.089849108367627</v>
-      </c>
-      <c r="AC4" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AD4" s="16">
-        <f t="shared" si="0"/>
-        <v>16.803840877914954</v>
-      </c>
-      <c r="AE4" s="17">
-        <v>0</v>
-      </c>
-      <c r="AF4" s="17">
-        <v>0</v>
-      </c>
-      <c r="AG4" s="17">
-        <v>0</v>
-      </c>
-      <c r="AH4" s="16">
-        <v>0</v>
-      </c>
-      <c r="AI4" s="17">
-        <v>0</v>
-      </c>
-      <c r="AJ4" s="17">
-        <v>0</v>
-      </c>
-      <c r="AK4" s="17">
-        <v>0</v>
-      </c>
-      <c r="AL4" s="17">
-        <v>0</v>
-      </c>
-      <c r="AM4" s="16">
-        <v>0</v>
-      </c>
-      <c r="AN4" s="17">
-        <v>0</v>
-      </c>
-      <c r="AO4" s="17">
-        <v>0</v>
-      </c>
-      <c r="AP4" s="17">
-        <v>0</v>
-      </c>
-      <c r="AQ4" s="17">
-        <v>0</v>
-      </c>
-      <c r="AR4" s="17">
-        <v>0</v>
-      </c>
-      <c r="AS4" s="17">
-        <v>0</v>
-      </c>
-      <c r="AT4" s="17">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFFF0000"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>99</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="6" tint="-0.249977111117893"/>
-  </sheetPr>
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="6" tint="-0.249977111117893"/>
-  </sheetPr>
-  <dimension ref="A1:G17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2753,6 +1947,724 @@
       </c>
       <c r="G17" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="6" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:H44"/>
+  <sheetViews>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="12"/>
+      <c r="H1" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="18">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="19">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>1.9E-2</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>0.01</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="14">
+        <v>-0.05</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>-0.04</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>0.06</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>0.06</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>0.02</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" s="2">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="2">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>0.01</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="4">
+        <v>3</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="15">
+        <v>-0.01</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14">
+        <v>0.01</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15">
+        <v>0.01</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16">
+        <v>0.01</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17">
+        <v>0.01</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18">
+        <v>0.01</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19">
+        <v>0.01</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="15">
+        <v>-0.01</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>0.01</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>0.01</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>0.01</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <v>0.01</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>0.01</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <v>0.01</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="F28" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="15">
+        <v>-0.01</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30">
+        <v>0.01</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>102</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31">
+        <v>0.01</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="F32" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E33" s="15">
+        <v>-0.01</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>106</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34">
+        <v>0.05</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E35">
+        <v>0.01</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>108</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E36">
+        <v>0.01</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" s="4"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="F37" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>110</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E38" s="15">
+        <v>-0.01</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>111</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E39">
+        <v>0.01</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>112</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40">
+        <v>0.01</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>113</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E41">
+        <v>0.01</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>114</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E42">
+        <v>0.01</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>115</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E43">
+        <v>0.01</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" s="4"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="F44" s="3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2766,12 +2678,11 @@
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2984,37 +2895,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" t="s">
-        <v>2</v>
-      </c>
-      <c r="F19" t="s">
-        <v>2</v>
-      </c>
-      <c r="G19" t="s">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3024,91 +2904,228 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor theme="6" tint="-0.249977111117893"/>
+    <tabColor theme="6" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>35</v>
       </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>36</v>
       </c>
-      <c r="B9">
-        <v>5</v>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3120,9 +3137,8 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -3163,7 +3179,7 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3171,7 +3187,7 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3179,7 +3195,7 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -3187,7 +3203,7 @@
         <v>35</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3195,7 +3211,7 @@
         <v>36</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -3205,12 +3221,104 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="6" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="0" tint="-4.9989318521683403E-2"/>
+  </sheetPr>
   <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3407,14 +3515,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="0" tint="-0.14999847407452621"/>
+  </sheetPr>
   <dimension ref="A1:AT3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3900,17 +4010,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor rgb="FFFF0000"/>
+    <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4034,408 +4143,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="6" tint="-0.249977111117893"/>
-  </sheetPr>
-  <dimension ref="A1:E43"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:F7"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="18">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="19">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="2">
-        <v>3</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="2">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="2">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" s="4">
-        <v>3</v>
-      </c>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="4"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="4"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>64</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>57</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C36" s="4"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>58</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>59</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>60</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>61</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>62</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C43" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
sii_debug() en ex5 toegevoegd
</commit_message>
<xml_diff>
--- a/xls/preparingtables.xlsx
+++ b/xls/preparingtables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="6420" windowWidth="28800" windowHeight="6480" tabRatio="904" activeTab="5"/>
+    <workbookView xWindow="-15" yWindow="6420" windowWidth="28800" windowHeight="6480" tabRatio="904" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="struct_sf16_eng" sheetId="8" r:id="rId1"/>
@@ -19,13 +19,14 @@
     <sheet name="ex3_data" sheetId="24" r:id="rId10"/>
     <sheet name="ex3_levelmax" sheetId="26" r:id="rId11"/>
     <sheet name="ex4_outline" sheetId="23" r:id="rId12"/>
+    <sheet name="ex5_data" sheetId="34" r:id="rId13"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="119">
   <si>
     <t>2d</t>
   </si>
@@ -261,9 +262,6 @@
     <t>SKV</t>
   </si>
   <si>
-    <t>KernSKV</t>
-  </si>
-  <si>
     <t>operationeel</t>
   </si>
   <si>
@@ -376,6 +374,15 @@
   </si>
   <si>
     <t>z_a_revisie</t>
+  </si>
+  <si>
+    <t>KSKV</t>
+  </si>
+  <si>
+    <t>tijd</t>
+  </si>
+  <si>
+    <t>vergelijkmet</t>
   </si>
 </sst>
 </file>
@@ -1986,6 +1993,501 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="0" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:AT3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4" style="10" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="4.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="4" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="4" style="10" bestFit="1" customWidth="1"/>
+    <col min="35" max="38" width="4" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="4" style="10" bestFit="1" customWidth="1"/>
+    <col min="40" max="46" width="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:46" ht="75.75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="9" t="str">
+        <f t="array" ref="E1:AT1">TRANSPOSE(struct_sf16_nld!A2:A44)</f>
+        <v>SKV</v>
+      </c>
+      <c r="F1" s="11" t="str">
+        <v>KSKV</v>
+      </c>
+      <c r="G1" s="8" t="str">
+        <v>operationeel</v>
+      </c>
+      <c r="H1" s="9" t="str">
+        <v>LACDT</v>
+      </c>
+      <c r="I1" s="8" t="str">
+        <v>KSKV-div</v>
+      </c>
+      <c r="J1" s="8" t="str">
+        <v>markt</v>
+      </c>
+      <c r="K1" s="8" t="str">
+        <v>leven</v>
+      </c>
+      <c r="L1" s="8" t="str">
+        <v>schade</v>
+      </c>
+      <c r="M1" s="8" t="str">
+        <v>zorg</v>
+      </c>
+      <c r="N1" s="8" t="str">
+        <v>tegenpartijkrediet</v>
+      </c>
+      <c r="O1" s="9" t="str">
+        <v>intangibles</v>
+      </c>
+      <c r="P1" s="8" t="str">
+        <v>markt-div</v>
+      </c>
+      <c r="Q1" s="8" t="str">
+        <v>m_rente</v>
+      </c>
+      <c r="R1" s="8" t="str">
+        <v>m_aandelen</v>
+      </c>
+      <c r="S1" s="8" t="str">
+        <v>m_vastgoed</v>
+      </c>
+      <c r="T1" s="8" t="str">
+        <v>m_spread</v>
+      </c>
+      <c r="U1" s="8" t="str">
+        <v>m_valuta</v>
+      </c>
+      <c r="V1" s="9" t="str">
+        <v>m_concentratie</v>
+      </c>
+      <c r="W1" s="8" t="str">
+        <v>m_illiquiditeit</v>
+      </c>
+      <c r="X1" s="8" t="str">
+        <v>leven-div</v>
+      </c>
+      <c r="Y1" s="8" t="str">
+        <v>l_kortleven</v>
+      </c>
+      <c r="Z1" s="8" t="str">
+        <v>l_langleven</v>
+      </c>
+      <c r="AA1" s="8" t="str">
+        <v>l_ao</v>
+      </c>
+      <c r="AB1" s="8" t="str">
+        <v>l_verval</v>
+      </c>
+      <c r="AC1" s="8" t="str">
+        <v>l_kosten</v>
+      </c>
+      <c r="AD1" s="9" t="str">
+        <v>l_revisie</v>
+      </c>
+      <c r="AE1" s="8" t="str">
+        <v>l_CAT</v>
+      </c>
+      <c r="AF1" s="8" t="str">
+        <v>schade-div</v>
+      </c>
+      <c r="AG1" s="8" t="str">
+        <v>s_premiereserve</v>
+      </c>
+      <c r="AH1" s="9" t="str">
+        <v>s_verval</v>
+      </c>
+      <c r="AI1" s="8" t="str">
+        <v>s_CAT</v>
+      </c>
+      <c r="AJ1" s="8" t="str">
+        <v>zorg-div</v>
+      </c>
+      <c r="AK1" s="8" t="str">
+        <v>z_alsleven</v>
+      </c>
+      <c r="AL1" s="8" t="str">
+        <v>z_CAT</v>
+      </c>
+      <c r="AM1" s="9" t="str">
+        <v>z_s_premiereserve</v>
+      </c>
+      <c r="AN1" s="8" t="str">
+        <v>z_s_verval</v>
+      </c>
+      <c r="AO1" s="8" t="str">
+        <v>z_alsleven-div</v>
+      </c>
+      <c r="AP1" s="8" t="str">
+        <v>z_a_kortleven</v>
+      </c>
+      <c r="AQ1" s="8" t="str">
+        <v>z_a_langleven</v>
+      </c>
+      <c r="AR1" s="8" t="str">
+        <v>z_a_ao</v>
+      </c>
+      <c r="AS1" s="8" t="str">
+        <v>z_a_verval</v>
+      </c>
+      <c r="AT1" s="8" t="str">
+        <v>z_a_kosten</v>
+      </c>
+    </row>
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A2" s="17">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17">
+        <v>1</v>
+      </c>
+      <c r="D2" s="17">
+        <v>230</v>
+      </c>
+      <c r="E2" s="16">
+        <v>91.8</v>
+      </c>
+      <c r="F2" s="17">
+        <v>113</v>
+      </c>
+      <c r="G2" s="17">
+        <v>7</v>
+      </c>
+      <c r="H2" s="16">
+        <v>-30.5</v>
+      </c>
+      <c r="I2" s="17">
+        <v>-31.4</v>
+      </c>
+      <c r="J2" s="17">
+        <v>64.2</v>
+      </c>
+      <c r="K2" s="17">
+        <v>80.2</v>
+      </c>
+      <c r="L2" s="17">
+        <v>0</v>
+      </c>
+      <c r="M2" s="17">
+        <v>0</v>
+      </c>
+      <c r="N2" s="17">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="O2" s="16">
+        <v>0</v>
+      </c>
+      <c r="P2" s="17">
+        <v>-4.7</v>
+      </c>
+      <c r="Q2" s="17">
+        <v>2.7</v>
+      </c>
+      <c r="R2" s="17">
+        <v>10.5</v>
+      </c>
+      <c r="S2" s="17">
+        <v>1.6</v>
+      </c>
+      <c r="T2" s="17">
+        <v>53.5</v>
+      </c>
+      <c r="U2" s="17">
+        <v>0.6</v>
+      </c>
+      <c r="V2" s="16">
+        <v>0</v>
+      </c>
+      <c r="W2" s="17">
+        <v>-44</v>
+      </c>
+      <c r="X2" s="17">
+        <v>29</v>
+      </c>
+      <c r="Y2" s="17">
+        <v>6.1</v>
+      </c>
+      <c r="Z2" s="17">
+        <v>0.4</v>
+      </c>
+      <c r="AA2" s="17">
+        <v>48</v>
+      </c>
+      <c r="AB2" s="17">
+        <v>21.1</v>
+      </c>
+      <c r="AC2" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="16">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="AE2" s="17">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="17">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="16">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="17">
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="17">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="17">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="17">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="16">
+        <v>0</v>
+      </c>
+      <c r="AN2" s="17">
+        <v>0</v>
+      </c>
+      <c r="AO2" s="17">
+        <v>0</v>
+      </c>
+      <c r="AP2" s="17">
+        <v>0</v>
+      </c>
+      <c r="AQ2" s="17">
+        <v>0</v>
+      </c>
+      <c r="AR2" s="17">
+        <v>0</v>
+      </c>
+      <c r="AS2" s="17">
+        <v>0</v>
+      </c>
+      <c r="AT2" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A3" s="17">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17">
+        <v>1</v>
+      </c>
+      <c r="C3" s="17">
+        <v>4</v>
+      </c>
+      <c r="D3" s="17">
+        <v>235</v>
+      </c>
+      <c r="E3" s="16">
+        <f>85/$E$2*E2</f>
+        <v>85</v>
+      </c>
+      <c r="F3" s="17">
+        <f t="shared" ref="F3:AD3" si="0">85/$E$2*F2</f>
+        <v>104.62962962962963</v>
+      </c>
+      <c r="G3" s="17">
+        <f t="shared" si="0"/>
+        <v>6.4814814814814818</v>
+      </c>
+      <c r="H3" s="16">
+        <f t="shared" si="0"/>
+        <v>-28.24074074074074</v>
+      </c>
+      <c r="I3" s="17">
+        <f t="shared" si="0"/>
+        <v>-29.074074074074073</v>
+      </c>
+      <c r="J3" s="17">
+        <f t="shared" si="0"/>
+        <v>59.44444444444445</v>
+      </c>
+      <c r="K3" s="17">
+        <f t="shared" si="0"/>
+        <v>74.259259259259267</v>
+      </c>
+      <c r="L3" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M3" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N3" s="17">
+        <f t="shared" si="0"/>
+        <v>2.1296296296296293</v>
+      </c>
+      <c r="O3" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P3" s="17">
+        <f t="shared" si="0"/>
+        <v>-4.3518518518518521</v>
+      </c>
+      <c r="Q3" s="17">
+        <f>85/$E$2*Q2+3</f>
+        <v>5.5</v>
+      </c>
+      <c r="R3" s="17">
+        <f>85/$E$2*R2+5</f>
+        <v>14.722222222222221</v>
+      </c>
+      <c r="S3" s="17">
+        <f>85/$E$2*S2+2</f>
+        <v>3.4814814814814818</v>
+      </c>
+      <c r="T3" s="17">
+        <f>85/$E$2*T2-10</f>
+        <v>39.537037037037038</v>
+      </c>
+      <c r="U3" s="17">
+        <f t="shared" si="0"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="V3" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W3" s="17">
+        <f t="shared" si="0"/>
+        <v>-40.74074074074074</v>
+      </c>
+      <c r="X3" s="17">
+        <f>85/$E$2*X2-3</f>
+        <v>23.851851851851851</v>
+      </c>
+      <c r="Y3" s="17">
+        <f>85/$E$2*Y2-1</f>
+        <v>4.6481481481481479</v>
+      </c>
+      <c r="Z3" s="17">
+        <f t="shared" si="0"/>
+        <v>0.37037037037037041</v>
+      </c>
+      <c r="AA3" s="17">
+        <f>85/$E$2*AA2+4</f>
+        <v>48.444444444444443</v>
+      </c>
+      <c r="AB3" s="17">
+        <f t="shared" si="0"/>
+        <v>19.537037037037038</v>
+      </c>
+      <c r="AC3" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD3" s="16">
+        <f t="shared" si="0"/>
+        <v>18.148148148148149</v>
+      </c>
+      <c r="AE3" s="17">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="17">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="17">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="16">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="17">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="17">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="17">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="17">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="16">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="17">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="17">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="17">
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="17">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="17">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="17">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="17">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
@@ -1993,8 +2495,8 @@
   </sheetPr>
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2049,7 +2551,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>116</v>
       </c>
       <c r="B3" s="19">
         <v>2</v>
@@ -2066,7 +2568,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" s="2">
         <v>2</v>
@@ -2080,7 +2582,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>0</v>
@@ -2096,7 +2598,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
@@ -2110,7 +2612,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" s="2">
         <v>3</v>
@@ -2127,7 +2629,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" s="2">
         <v>3</v>
@@ -2144,7 +2646,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9" s="2">
         <v>3</v>
@@ -2161,7 +2663,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B10" s="2">
         <v>3</v>
@@ -2178,7 +2680,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B11" s="2">
         <v>3</v>
@@ -2208,7 +2710,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>11</v>
@@ -2222,7 +2724,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>9</v>
@@ -2236,7 +2738,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>9</v>
@@ -2250,7 +2752,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>9</v>
@@ -2278,7 +2780,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>9</v>
@@ -2292,7 +2794,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>9</v>
@@ -2306,7 +2808,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>9</v>
@@ -2322,7 +2824,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>8</v>
@@ -2336,7 +2838,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>3</v>
@@ -2350,7 +2852,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>3</v>
@@ -2364,7 +2866,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>3</v>
@@ -2378,7 +2880,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>3</v>
@@ -2392,7 +2894,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>3</v>
@@ -2406,7 +2908,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>3</v>
@@ -2436,7 +2938,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>6</v>
@@ -2450,7 +2952,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>4</v>
@@ -2464,7 +2966,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>4</v>
@@ -2478,7 +2980,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>4</v>
@@ -2494,7 +2996,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>65</v>
@@ -2508,7 +3010,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>35</v>
@@ -2525,7 +3027,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>35</v>
@@ -2539,7 +3041,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>35</v>
@@ -2553,7 +3055,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>35</v>
@@ -2569,7 +3071,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>71</v>
@@ -2583,7 +3085,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>36</v>
@@ -2597,7 +3099,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>36</v>
@@ -2611,7 +3113,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>36</v>
@@ -2625,7 +3127,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>36</v>
@@ -2639,7 +3141,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>36</v>
@@ -2653,7 +3155,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>36</v>
@@ -3079,7 +3581,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B16" t="s">
         <v>72</v>
@@ -3102,7 +3604,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B17" t="s">
         <v>72</v>
@@ -3226,7 +3728,7 @@
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -3523,7 +4025,7 @@
   <dimension ref="A1:AT3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
hernoemen fnX naar fn_x uitgebreide voorbeeldenset maken met aanpassen data
</commit_message>
<xml_diff>
--- a/xls/preparingtables.xlsx
+++ b/xls/preparingtables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="6420" windowWidth="28800" windowHeight="6480" tabRatio="904" activeTab="12"/>
+    <workbookView xWindow="-15" yWindow="6420" windowWidth="28800" windowHeight="6480" tabRatio="904" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="struct_sf16_eng" sheetId="8" r:id="rId1"/>
@@ -2000,7 +2000,7 @@
   </sheetPr>
   <dimension ref="A1:AT3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3819,7 +3819,7 @@
   <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3827,17 +3827,16 @@
     <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.28515625" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="4" bestFit="1" customWidth="1"/>
@@ -3942,73 +3941,73 @@
         <v>230</v>
       </c>
       <c r="D2" s="16">
-        <v>66.099999999999994</v>
+        <v>30</v>
       </c>
       <c r="E2" s="17">
-        <v>81.400000000000006</v>
+        <v>35</v>
       </c>
       <c r="F2" s="17">
         <v>5</v>
       </c>
       <c r="G2" s="16">
-        <v>-22</v>
+        <v>-10</v>
       </c>
       <c r="H2" s="17">
-        <v>-22.6</v>
+        <v>-5</v>
       </c>
       <c r="I2" s="17">
-        <v>46.2</v>
+        <v>20</v>
       </c>
       <c r="J2" s="16">
-        <v>57.8</v>
+        <v>15</v>
       </c>
       <c r="K2" s="16">
-        <v>1.7</v>
+        <v>5</v>
       </c>
       <c r="L2" s="17">
-        <v>-3.4</v>
+        <v>-30</v>
       </c>
       <c r="M2" s="17">
-        <v>1.9</v>
+        <v>8</v>
       </c>
       <c r="N2" s="17">
-        <v>7.6</v>
+        <v>7</v>
       </c>
       <c r="O2" s="17">
-        <v>1.2</v>
+        <v>6</v>
       </c>
       <c r="P2" s="17">
-        <v>38.5</v>
+        <v>6</v>
       </c>
       <c r="Q2" s="17">
-        <v>0.4</v>
+        <v>5</v>
       </c>
       <c r="R2" s="16">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S2" s="17">
-        <v>-31.7</v>
+        <v>-4</v>
       </c>
       <c r="T2" s="17">
-        <v>20.9</v>
+        <v>1</v>
       </c>
       <c r="U2" s="17">
-        <v>4.4000000000000004</v>
+        <v>2</v>
       </c>
       <c r="V2" s="17">
-        <v>0.3</v>
+        <v>3</v>
       </c>
       <c r="W2" s="17">
-        <v>34.6</v>
+        <v>5</v>
       </c>
       <c r="X2" s="17">
-        <v>15.2</v>
+        <v>4</v>
       </c>
       <c r="Y2" s="17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z2" s="16">
-        <v>14.1</v>
+        <v>2</v>
       </c>
       <c r="AA2" s="17"/>
     </row>
@@ -4022,17 +4021,17 @@
   <sheetPr>
     <tabColor theme="0" tint="-0.14999847407452621"/>
   </sheetPr>
-  <dimension ref="A1:AT3"/>
+  <dimension ref="A1:AT4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
@@ -4209,7 +4208,7 @@
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17">
-        <v>1</v>
+        <v>2017</v>
       </c>
       <c r="D2" s="17">
         <v>230</v>
@@ -4349,17 +4348,17 @@
         <v>1</v>
       </c>
       <c r="C3" s="17">
-        <v>4</v>
+        <v>2021</v>
       </c>
       <c r="D3" s="17">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E3" s="16">
         <f>85/$E$2*E2</f>
         <v>85</v>
       </c>
       <c r="F3" s="17">
-        <f t="shared" ref="F3:AD3" si="0">85/$E$2*F2</f>
+        <f t="shared" ref="F3:AD4" si="0">85/$E$2*F2</f>
         <v>104.62962962962963</v>
       </c>
       <c r="G3" s="17">
@@ -4505,6 +4504,161 @@
       </c>
       <c r="AT3" s="17">
         <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2021</v>
+      </c>
+      <c r="D4">
+        <v>228</v>
+      </c>
+      <c r="E4" s="10">
+        <v>145</v>
+      </c>
+      <c r="F4" s="20">
+        <v>160</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4" s="10">
+        <v>-20</v>
+      </c>
+      <c r="I4">
+        <v>-27.4</v>
+      </c>
+      <c r="J4" s="17">
+        <v>64.2</v>
+      </c>
+      <c r="K4" s="17">
+        <v>80.2</v>
+      </c>
+      <c r="L4">
+        <v>6</v>
+      </c>
+      <c r="M4">
+        <v>35</v>
+      </c>
+      <c r="N4">
+        <v>2</v>
+      </c>
+      <c r="O4" s="10">
+        <v>0</v>
+      </c>
+      <c r="P4" s="17">
+        <f t="shared" si="0"/>
+        <v>-4.0294924554183815</v>
+      </c>
+      <c r="Q4" s="17">
+        <f>85/$E$2*Q3+3</f>
+        <v>8.0925925925925917</v>
+      </c>
+      <c r="R4" s="17">
+        <f>85/$E$2*R3+5</f>
+        <v>18.631687242798353</v>
+      </c>
+      <c r="S4" s="17">
+        <f>85/$E$2*S3+2</f>
+        <v>5.2235939643347056</v>
+      </c>
+      <c r="T4" s="17">
+        <f>85/$E$2*T3-10</f>
+        <v>26.60836762688615</v>
+      </c>
+      <c r="U4" s="17">
+        <f t="shared" si="0"/>
+        <v>0.51440329218106995</v>
+      </c>
+      <c r="V4" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W4" s="17">
+        <f t="shared" si="0"/>
+        <v>-37.722908093278463</v>
+      </c>
+      <c r="X4" s="17">
+        <f>85/$E$2*X3-3</f>
+        <v>19.085048010973935</v>
+      </c>
+      <c r="Y4" s="17">
+        <f>85/$E$2*Y3-1</f>
+        <v>3.3038408779149515</v>
+      </c>
+      <c r="Z4" s="17">
+        <f t="shared" si="0"/>
+        <v>0.34293552812071332</v>
+      </c>
+      <c r="AA4" s="17">
+        <f>85/$E$2*AA3+4</f>
+        <v>48.855967078189302</v>
+      </c>
+      <c r="AB4" s="17">
+        <f t="shared" si="0"/>
+        <v>18.089849108367627</v>
+      </c>
+      <c r="AC4" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD4" s="16">
+        <f t="shared" si="0"/>
+        <v>16.803840877914954</v>
+      </c>
+      <c r="AE4">
+        <v>0.2</v>
+      </c>
+      <c r="AF4">
+        <v>-1</v>
+      </c>
+      <c r="AG4">
+        <v>2</v>
+      </c>
+      <c r="AH4" s="10">
+        <v>4</v>
+      </c>
+      <c r="AI4">
+        <v>1</v>
+      </c>
+      <c r="AJ4">
+        <v>-8</v>
+      </c>
+      <c r="AK4">
+        <v>25</v>
+      </c>
+      <c r="AL4">
+        <v>4</v>
+      </c>
+      <c r="AM4" s="10">
+        <v>6</v>
+      </c>
+      <c r="AN4" s="20">
+        <v>8</v>
+      </c>
+      <c r="AO4" s="20">
+        <v>-5</v>
+      </c>
+      <c r="AP4">
+        <v>2</v>
+      </c>
+      <c r="AQ4">
+        <v>4</v>
+      </c>
+      <c r="AR4">
+        <v>6</v>
+      </c>
+      <c r="AS4">
+        <v>8</v>
+      </c>
+      <c r="AT4">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
content example2_data gecorrigeerd ordering levels tbv legenda ingesteld
</commit_message>
<xml_diff>
--- a/xls/preparingtables.xlsx
+++ b/xls/preparingtables.xlsx
@@ -392,7 +392,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,8 +408,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -422,8 +429,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -458,11 +471,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -503,12 +525,47 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFF99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -4021,10 +4078,10 @@
   <sheetPr>
     <tabColor theme="0" tint="-0.14999847407452621"/>
   </sheetPr>
-  <dimension ref="A1:AT4"/>
+  <dimension ref="A1:AT5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4033,32 +4090,33 @@
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4" style="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4" style="10" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="4.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="31" max="33" width="4" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="4" style="10" bestFit="1" customWidth="1"/>
-    <col min="35" max="38" width="4" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="4" style="10" bestFit="1" customWidth="1"/>
-    <col min="40" max="46" width="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="5.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4" style="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" style="32" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" style="24" customWidth="1"/>
+    <col min="13" max="15" width="4" style="24" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4" style="24" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4" style="24" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="4" style="24" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="4" style="24" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="4.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="4" style="24" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="4.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="4" style="24" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4" style="30" bestFit="1" customWidth="1"/>
+    <col min="33" max="35" width="4" style="24" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="4" style="30" bestFit="1" customWidth="1"/>
+    <col min="37" max="40" width="4" style="24" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="4" style="30" bestFit="1" customWidth="1"/>
+    <col min="42" max="46" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46" ht="75.75" x14ac:dyDescent="0.25">
@@ -4074,116 +4132,116 @@
       <c r="D1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="9" t="str">
+      <c r="E1" s="25" t="str">
         <f t="array" ref="E1:AT1">TRANSPOSE(struct_sf16_eng!A2:A44)</f>
         <v>SCR</v>
       </c>
-      <c r="F1" s="11" t="str">
+      <c r="F1" s="28" t="str">
         <v>BSCR</v>
       </c>
-      <c r="G1" s="8" t="str">
+      <c r="G1" s="22" t="str">
         <v>operational</v>
       </c>
-      <c r="H1" s="9" t="str">
+      <c r="H1" s="31" t="str">
         <v>Adjustment-LACDT</v>
       </c>
-      <c r="I1" s="8" t="str">
+      <c r="I1" s="29" t="str">
         <v>BSCR_div</v>
       </c>
-      <c r="J1" s="8" t="str">
+      <c r="J1" s="22" t="str">
         <v>market</v>
       </c>
-      <c r="K1" s="8" t="str">
+      <c r="K1" s="22" t="str">
         <v>life</v>
       </c>
-      <c r="L1" s="8" t="str">
+      <c r="L1" s="22" t="str">
         <v>nonlife</v>
       </c>
-      <c r="M1" s="8" t="str">
+      <c r="M1" s="22" t="str">
         <v>health</v>
       </c>
-      <c r="N1" s="8" t="str">
+      <c r="N1" s="22" t="str">
         <v>cp-default</v>
       </c>
-      <c r="O1" s="9" t="str">
+      <c r="O1" s="22" t="str">
         <v>intangibles</v>
       </c>
-      <c r="P1" s="8" t="str">
+      <c r="P1" s="29" t="str">
         <v>market_div</v>
       </c>
-      <c r="Q1" s="8" t="str">
+      <c r="Q1" s="22" t="str">
         <v>m_interestrate</v>
       </c>
-      <c r="R1" s="8" t="str">
+      <c r="R1" s="22" t="str">
         <v>m_equity</v>
       </c>
-      <c r="S1" s="8" t="str">
+      <c r="S1" s="22" t="str">
         <v>m_property</v>
       </c>
-      <c r="T1" s="8" t="str">
+      <c r="T1" s="22" t="str">
         <v>m_spread</v>
       </c>
-      <c r="U1" s="8" t="str">
+      <c r="U1" s="22" t="str">
         <v>m_currency</v>
       </c>
-      <c r="V1" s="9" t="str">
+      <c r="V1" s="22" t="str">
         <v>m_concentration</v>
       </c>
-      <c r="W1" s="8" t="str">
+      <c r="W1" s="22" t="str">
         <v>m_illiquidity</v>
       </c>
-      <c r="X1" s="8" t="str">
+      <c r="X1" s="29" t="str">
         <v>life_div</v>
       </c>
-      <c r="Y1" s="8" t="str">
+      <c r="Y1" s="22" t="str">
         <v>l_mortality</v>
       </c>
-      <c r="Z1" s="8" t="str">
+      <c r="Z1" s="22" t="str">
         <v>l_longevity</v>
       </c>
-      <c r="AA1" s="8" t="str">
+      <c r="AA1" s="22" t="str">
         <v>l_disability</v>
       </c>
-      <c r="AB1" s="8" t="str">
+      <c r="AB1" s="22" t="str">
         <v>l_lapse</v>
       </c>
-      <c r="AC1" s="8" t="str">
+      <c r="AC1" s="22" t="str">
         <v>l_expenses</v>
       </c>
-      <c r="AD1" s="9" t="str">
+      <c r="AD1" s="22" t="str">
         <v>l_revision</v>
       </c>
-      <c r="AE1" s="8" t="str">
+      <c r="AE1" s="22" t="str">
         <v>l_CAT</v>
       </c>
-      <c r="AF1" s="8" t="str">
+      <c r="AF1" s="29" t="str">
         <v>nonlife_div</v>
       </c>
-      <c r="AG1" s="8" t="str">
+      <c r="AG1" s="22" t="str">
         <v>n_premiumreserve</v>
       </c>
-      <c r="AH1" s="9" t="str">
+      <c r="AH1" s="22" t="str">
         <v>n_lapse</v>
       </c>
-      <c r="AI1" s="8" t="str">
+      <c r="AI1" s="22" t="str">
         <v>n_CAT</v>
       </c>
-      <c r="AJ1" s="8" t="str">
+      <c r="AJ1" s="29" t="str">
         <v>health_div</v>
       </c>
-      <c r="AK1" s="8" t="str">
+      <c r="AK1" s="22" t="str">
         <v>h_SLT</v>
       </c>
-      <c r="AL1" s="8" t="str">
+      <c r="AL1" s="22" t="str">
         <v>h_CAT</v>
       </c>
-      <c r="AM1" s="9" t="str">
+      <c r="AM1" s="22" t="str">
         <v>h_n_premiumres</v>
       </c>
-      <c r="AN1" s="8" t="str">
+      <c r="AN1" s="22" t="str">
         <v>h_n_lapse</v>
       </c>
-      <c r="AO1" s="8" t="str">
+      <c r="AO1" s="29" t="str">
         <v>h_SLT_div</v>
       </c>
       <c r="AP1" s="8" t="str">
@@ -4213,130 +4271,137 @@
       <c r="D2" s="17">
         <v>230</v>
       </c>
-      <c r="E2" s="16">
-        <v>91.8</v>
-      </c>
-      <c r="F2" s="17">
-        <v>113</v>
-      </c>
-      <c r="G2" s="17">
+      <c r="E2" s="26">
+        <f>SUM(F2:H2)</f>
+        <v>139.80000000000001</v>
+      </c>
+      <c r="F2" s="26">
+        <f>SUM(I2:O2)</f>
+        <v>163.30000000000001</v>
+      </c>
+      <c r="G2" s="33">
         <v>7</v>
       </c>
-      <c r="H2" s="16">
+      <c r="H2" s="39">
         <v>-30.5</v>
       </c>
-      <c r="I2" s="17">
+      <c r="I2" s="35">
         <v>-31.4</v>
       </c>
-      <c r="J2" s="17">
-        <v>64.2</v>
-      </c>
-      <c r="K2" s="17">
-        <v>80.2</v>
-      </c>
-      <c r="L2" s="17">
-        <v>0</v>
-      </c>
-      <c r="M2" s="17">
-        <v>0</v>
-      </c>
-      <c r="N2" s="17">
+      <c r="J2" s="23">
+        <f>SUM(P2:W2)</f>
+        <v>68.2</v>
+      </c>
+      <c r="K2" s="23">
+        <f>SUM(X2:AE2)</f>
+        <v>124.19999999999999</v>
+      </c>
+      <c r="L2" s="23">
+        <f>SUM(AF2:AI2)</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="24">
+        <f>SUM(AJ2:AN2)</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="33">
         <v>2.2999999999999998</v>
       </c>
-      <c r="O2" s="16">
-        <v>0</v>
-      </c>
-      <c r="P2" s="17">
+      <c r="O2" s="33">
+        <v>0</v>
+      </c>
+      <c r="P2" s="35">
         <v>-4.7</v>
       </c>
-      <c r="Q2" s="17">
+      <c r="Q2" s="33">
         <v>2.7</v>
       </c>
-      <c r="R2" s="17">
+      <c r="R2" s="33">
         <v>10.5</v>
       </c>
-      <c r="S2" s="17">
+      <c r="S2" s="33">
         <v>1.6</v>
       </c>
-      <c r="T2" s="17">
+      <c r="T2" s="33">
         <v>53.5</v>
       </c>
-      <c r="U2" s="17">
+      <c r="U2" s="33">
         <v>0.6</v>
       </c>
-      <c r="V2" s="16">
-        <v>0</v>
-      </c>
-      <c r="W2" s="17">
-        <v>-44</v>
-      </c>
-      <c r="X2" s="17">
+      <c r="V2" s="33">
+        <v>0</v>
+      </c>
+      <c r="W2" s="33">
+        <v>4</v>
+      </c>
+      <c r="X2" s="35">
         <v>29</v>
       </c>
-      <c r="Y2" s="17">
+      <c r="Y2" s="33">
         <v>6.1</v>
       </c>
-      <c r="Z2" s="17">
+      <c r="Z2" s="33">
         <v>0.4</v>
       </c>
-      <c r="AA2" s="17">
+      <c r="AA2" s="33">
         <v>48</v>
       </c>
-      <c r="AB2" s="17">
+      <c r="AB2" s="33">
         <v>21.1</v>
       </c>
-      <c r="AC2" s="17">
-        <v>0</v>
-      </c>
-      <c r="AD2" s="16">
+      <c r="AC2" s="33">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="33">
         <v>19.600000000000001</v>
       </c>
-      <c r="AE2" s="17">
-        <v>0</v>
-      </c>
-      <c r="AF2" s="17">
-        <v>0</v>
-      </c>
-      <c r="AG2" s="17">
-        <v>0</v>
-      </c>
-      <c r="AH2" s="16">
-        <v>0</v>
-      </c>
-      <c r="AI2" s="17">
-        <v>0</v>
-      </c>
-      <c r="AJ2" s="17">
-        <v>0</v>
-      </c>
-      <c r="AK2" s="17">
-        <v>0</v>
-      </c>
-      <c r="AL2" s="17">
-        <v>0</v>
-      </c>
-      <c r="AM2" s="16">
-        <v>0</v>
-      </c>
-      <c r="AN2" s="17">
-        <v>0</v>
-      </c>
-      <c r="AO2" s="17">
-        <v>0</v>
-      </c>
-      <c r="AP2" s="17">
-        <v>0</v>
-      </c>
-      <c r="AQ2" s="17">
-        <v>0</v>
-      </c>
-      <c r="AR2" s="17">
-        <v>0</v>
-      </c>
-      <c r="AS2" s="17">
-        <v>0</v>
-      </c>
-      <c r="AT2" s="17">
+      <c r="AE2" s="33">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="35">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="33">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="33">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="33">
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="35">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="24">
+        <f>SUM(AO2:AT2)</f>
+        <v>0</v>
+      </c>
+      <c r="AL2" s="33">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="33">
+        <v>0</v>
+      </c>
+      <c r="AN2" s="33">
+        <v>0</v>
+      </c>
+      <c r="AO2" s="35">
+        <v>0</v>
+      </c>
+      <c r="AP2" s="36">
+        <v>0</v>
+      </c>
+      <c r="AQ2" s="36">
+        <v>0</v>
+      </c>
+      <c r="AR2" s="36">
+        <v>0</v>
+      </c>
+      <c r="AS2" s="36">
+        <v>0</v>
+      </c>
+      <c r="AT2" s="36">
         <v>0</v>
       </c>
     </row>
@@ -4353,156 +4418,156 @@
       <c r="D3" s="17">
         <v>234</v>
       </c>
-      <c r="E3" s="16">
-        <f>85/$E$2*E2</f>
-        <v>85</v>
-      </c>
-      <c r="F3" s="17">
-        <f t="shared" ref="F3:AD4" si="0">85/$E$2*F2</f>
-        <v>104.62962962962963</v>
-      </c>
-      <c r="G3" s="17">
+      <c r="E3" s="26">
+        <f>SUM(F3:H3)</f>
+        <v>89.567954220314746</v>
+      </c>
+      <c r="F3" s="26">
+        <f>SUM(I3:O3)</f>
+        <v>103.85622317596567</v>
+      </c>
+      <c r="G3" s="33">
+        <f t="shared" ref="F3:AD5" si="0">85/$E$2*G2</f>
+        <v>4.2560801144492126</v>
+      </c>
+      <c r="H3" s="39">
         <f t="shared" si="0"/>
-        <v>6.4814814814814818</v>
-      </c>
-      <c r="H3" s="16">
+        <v>-18.544349070100139</v>
+      </c>
+      <c r="I3" s="35">
         <f t="shared" si="0"/>
-        <v>-28.24074074074074</v>
-      </c>
-      <c r="I3" s="17">
+        <v>-19.091559370529325</v>
+      </c>
+      <c r="J3" s="23">
+        <f>SUM(P3:W3)</f>
+        <v>46.034334763948493</v>
+      </c>
+      <c r="K3" s="23">
+        <f>SUM(X3:AE3)</f>
+        <v>75.515021459227469</v>
+      </c>
+      <c r="L3" s="23">
+        <f>SUM(AF3:AI3)</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="24">
+        <f>SUM(AJ3:AN3)</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="33">
         <f t="shared" si="0"/>
-        <v>-29.074074074074073</v>
-      </c>
-      <c r="J3" s="17">
+        <v>1.3984263233190268</v>
+      </c>
+      <c r="O3" s="33">
         <f t="shared" si="0"/>
-        <v>59.44444444444445</v>
-      </c>
-      <c r="K3" s="17">
+        <v>0</v>
+      </c>
+      <c r="P3" s="35">
         <f t="shared" si="0"/>
-        <v>74.259259259259267</v>
-      </c>
-      <c r="L3" s="17">
+        <v>-2.8576537911301858</v>
+      </c>
+      <c r="Q3" s="33">
+        <f>85/$E$2*Q2+3</f>
+        <v>4.6416309012875541</v>
+      </c>
+      <c r="R3" s="33">
+        <f>85/$E$2*R2+5</f>
+        <v>11.384120171673819</v>
+      </c>
+      <c r="S3" s="33">
+        <f>85/$E$2*S2+2</f>
+        <v>2.9728183118741058</v>
+      </c>
+      <c r="T3" s="33">
+        <f>85/$E$2*T2-10</f>
+        <v>22.528612303290409</v>
+      </c>
+      <c r="U3" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M3" s="17">
+        <v>0.36480686695278963</v>
+      </c>
+      <c r="V3" s="33">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N3" s="17">
+      <c r="W3" s="33">
+        <v>7</v>
+      </c>
+      <c r="X3" s="35">
+        <f>85/$E$2*X2-3</f>
+        <v>14.632331902718168</v>
+      </c>
+      <c r="Y3" s="33">
+        <f>85/$E$2*Y2-1</f>
+        <v>2.7088698140200278</v>
+      </c>
+      <c r="Z3" s="33">
         <f t="shared" si="0"/>
-        <v>2.1296296296296293</v>
-      </c>
-      <c r="O3" s="16">
+        <v>0.24320457796852646</v>
+      </c>
+      <c r="AA3" s="33">
+        <f>85/$E$2*AA2+4</f>
+        <v>33.184549356223172</v>
+      </c>
+      <c r="AB3" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P3" s="17">
+        <v>12.82904148783977</v>
+      </c>
+      <c r="AC3" s="33">
         <f t="shared" si="0"/>
-        <v>-4.3518518518518521</v>
-      </c>
-      <c r="Q3" s="17">
-        <f>85/$E$2*Q2+3</f>
-        <v>5.5</v>
-      </c>
-      <c r="R3" s="17">
-        <f>85/$E$2*R2+5</f>
-        <v>14.722222222222221</v>
-      </c>
-      <c r="S3" s="17">
-        <f>85/$E$2*S2+2</f>
-        <v>3.4814814814814818</v>
-      </c>
-      <c r="T3" s="17">
-        <f>85/$E$2*T2-10</f>
-        <v>39.537037037037038</v>
-      </c>
-      <c r="U3" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="33">
         <f t="shared" si="0"/>
-        <v>0.55555555555555558</v>
-      </c>
-      <c r="V3" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W3" s="17">
-        <f t="shared" si="0"/>
-        <v>-40.74074074074074</v>
-      </c>
-      <c r="X3" s="17">
-        <f>85/$E$2*X2-3</f>
-        <v>23.851851851851851</v>
-      </c>
-      <c r="Y3" s="17">
-        <f>85/$E$2*Y2-1</f>
-        <v>4.6481481481481479</v>
-      </c>
-      <c r="Z3" s="17">
-        <f t="shared" si="0"/>
-        <v>0.37037037037037041</v>
-      </c>
-      <c r="AA3" s="17">
-        <f>85/$E$2*AA2+4</f>
-        <v>48.444444444444443</v>
-      </c>
-      <c r="AB3" s="17">
-        <f t="shared" si="0"/>
-        <v>19.537037037037038</v>
-      </c>
-      <c r="AC3" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AD3" s="16">
-        <f t="shared" si="0"/>
-        <v>18.148148148148149</v>
-      </c>
-      <c r="AE3" s="17">
-        <v>0</v>
-      </c>
-      <c r="AF3" s="17">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="17">
-        <v>0</v>
-      </c>
-      <c r="AH3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="17">
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="17">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="17">
-        <v>0</v>
-      </c>
-      <c r="AL3" s="17">
-        <v>0</v>
-      </c>
-      <c r="AM3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AN3" s="17">
-        <v>0</v>
-      </c>
-      <c r="AO3" s="17">
-        <v>0</v>
-      </c>
-      <c r="AP3" s="17">
-        <v>0</v>
-      </c>
-      <c r="AQ3" s="17">
-        <v>0</v>
-      </c>
-      <c r="AR3" s="17">
-        <v>0</v>
-      </c>
-      <c r="AS3" s="17">
-        <v>0</v>
-      </c>
-      <c r="AT3" s="17">
+        <v>11.917024320457797</v>
+      </c>
+      <c r="AE3" s="33">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="35">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="33">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="33">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="33">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="35">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="24">
+        <f>SUM(AO3:AT3)</f>
+        <v>0</v>
+      </c>
+      <c r="AL3" s="33">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="33">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="33">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="35">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="36">
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="36">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="36">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="36">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="36">
         <v>0</v>
       </c>
     </row>
@@ -4519,146 +4584,295 @@
       <c r="D4">
         <v>228</v>
       </c>
-      <c r="E4" s="10">
-        <v>145</v>
-      </c>
-      <c r="F4" s="20">
-        <v>160</v>
-      </c>
-      <c r="G4">
+      <c r="E4" s="26">
+        <f>SUM(F4:H4)</f>
+        <v>76.44731959205977</v>
+      </c>
+      <c r="F4" s="26">
+        <f>SUM(I4:O4)</f>
+        <v>91.44731959205977</v>
+      </c>
+      <c r="G4" s="34">
         <v>5</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="40">
         <v>-20</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="37">
         <v>-27.4</v>
       </c>
-      <c r="J4" s="17">
-        <v>64.2</v>
-      </c>
-      <c r="K4" s="17">
-        <v>80.2</v>
-      </c>
-      <c r="L4">
+      <c r="J4" s="23">
+        <f>SUM(P4:W4)</f>
+        <v>29.733322281370679</v>
+      </c>
+      <c r="K4" s="23">
+        <f>SUM(X4:AE4)</f>
+        <v>46.113997310689086</v>
+      </c>
+      <c r="L4" s="23">
+        <f>SUM(AF4:AI4)</f>
         <v>6</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="24">
+        <f>SUM(AJ4:AN4)</f>
         <v>35</v>
       </c>
-      <c r="N4">
-        <v>2</v>
-      </c>
-      <c r="O4" s="10">
-        <v>0</v>
-      </c>
-      <c r="P4" s="17">
+      <c r="N4" s="34">
+        <v>2</v>
+      </c>
+      <c r="O4" s="34">
+        <v>0</v>
+      </c>
+      <c r="P4" s="35">
         <f t="shared" si="0"/>
-        <v>-4.0294924554183815</v>
-      </c>
-      <c r="Q4" s="17">
+        <v>-1.7374862106299411</v>
+      </c>
+      <c r="Q4" s="33">
         <f>85/$E$2*Q3+3</f>
-        <v>8.0925925925925917</v>
-      </c>
-      <c r="R4" s="17">
+        <v>5.8221647110832766</v>
+      </c>
+      <c r="R4" s="41">
         <f>85/$E$2*R3+5</f>
-        <v>18.631687242798353</v>
-      </c>
-      <c r="S4" s="17">
+        <v>11.9216753547373</v>
+      </c>
+      <c r="S4" s="33">
         <f>85/$E$2*S3+2</f>
-        <v>5.2235939643347056</v>
-      </c>
-      <c r="T4" s="17">
+        <v>3.8075075572911228</v>
+      </c>
+      <c r="T4" s="41">
         <f>85/$E$2*T3-10</f>
-        <v>26.60836762688615</v>
-      </c>
-      <c r="U4" s="17">
+        <v>3.6976541185957394</v>
+      </c>
+      <c r="U4" s="33">
         <f t="shared" si="0"/>
-        <v>0.51440329218106995</v>
-      </c>
-      <c r="V4" s="16">
+        <v>0.22180675029318395</v>
+      </c>
+      <c r="V4" s="33">
+        <v>1</v>
+      </c>
+      <c r="W4" s="33">
+        <v>5</v>
+      </c>
+      <c r="X4" s="35">
+        <f>85/$E$2*X3-3</f>
+        <v>5.8966252627399438</v>
+      </c>
+      <c r="Y4" s="33">
+        <f>85/$E$2*Y3-1</f>
+        <v>0.64702384972605387</v>
+      </c>
+      <c r="Z4" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W4" s="17">
+        <v>0.14787116686212265</v>
+      </c>
+      <c r="AA4" s="33">
+        <f>85/$E$2*AA3+4</f>
+        <v>24.176585803139982</v>
+      </c>
+      <c r="AB4" s="33">
         <f t="shared" si="0"/>
-        <v>-37.722908093278463</v>
-      </c>
-      <c r="X4" s="17">
-        <f>85/$E$2*X3-3</f>
-        <v>19.085048010973935</v>
-      </c>
-      <c r="Y4" s="17">
-        <f>85/$E$2*Y3-1</f>
-        <v>3.3038408779149515</v>
-      </c>
-      <c r="Z4" s="17">
+        <v>7.8002040519769693</v>
+      </c>
+      <c r="AC4" s="33">
         <f t="shared" si="0"/>
-        <v>0.34293552812071332</v>
-      </c>
-      <c r="AA4" s="17">
-        <f>85/$E$2*AA3+4</f>
-        <v>48.855967078189302</v>
-      </c>
-      <c r="AB4" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="33">
         <f t="shared" si="0"/>
-        <v>18.089849108367627</v>
-      </c>
-      <c r="AC4" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AD4" s="16">
-        <f t="shared" si="0"/>
-        <v>16.803840877914954</v>
-      </c>
-      <c r="AE4">
+        <v>7.2456871762440098</v>
+      </c>
+      <c r="AE4" s="34">
         <v>0.2</v>
       </c>
-      <c r="AF4">
+      <c r="AF4" s="37">
         <v>-1</v>
       </c>
-      <c r="AG4">
-        <v>2</v>
-      </c>
-      <c r="AH4" s="10">
+      <c r="AG4" s="34">
+        <v>2</v>
+      </c>
+      <c r="AH4" s="34">
         <v>4</v>
       </c>
-      <c r="AI4">
-        <v>1</v>
-      </c>
-      <c r="AJ4">
+      <c r="AI4" s="34">
+        <v>1</v>
+      </c>
+      <c r="AJ4" s="37">
         <v>-8</v>
       </c>
-      <c r="AK4">
+      <c r="AK4" s="24">
+        <f>SUM(AO4:AT4)</f>
         <v>25</v>
       </c>
-      <c r="AL4">
+      <c r="AL4" s="34">
         <v>4</v>
       </c>
-      <c r="AM4" s="10">
+      <c r="AM4" s="34">
         <v>6</v>
       </c>
-      <c r="AN4" s="20">
+      <c r="AN4" s="34">
         <v>8</v>
       </c>
-      <c r="AO4" s="20">
+      <c r="AO4" s="37">
         <v>-5</v>
       </c>
-      <c r="AP4">
-        <v>2</v>
-      </c>
-      <c r="AQ4">
+      <c r="AP4" s="38">
+        <v>2</v>
+      </c>
+      <c r="AQ4" s="38">
         <v>4</v>
       </c>
-      <c r="AR4">
+      <c r="AR4" s="38">
         <v>6</v>
       </c>
-      <c r="AS4">
+      <c r="AS4" s="38">
         <v>8</v>
       </c>
-      <c r="AT4">
+      <c r="AT4" s="38">
         <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>2023</v>
+      </c>
+      <c r="D5">
+        <v>228</v>
+      </c>
+      <c r="E5" s="26">
+        <f>SUM(F5:H5)</f>
+        <v>80</v>
+      </c>
+      <c r="F5" s="26">
+        <f>SUM(I5:O5)</f>
+        <v>75</v>
+      </c>
+      <c r="G5" s="34">
+        <v>25</v>
+      </c>
+      <c r="H5" s="40">
+        <v>-20</v>
+      </c>
+      <c r="I5" s="37">
+        <v>-9</v>
+      </c>
+      <c r="J5" s="23">
+        <f>SUM(P5:W5)</f>
+        <v>14</v>
+      </c>
+      <c r="K5" s="23">
+        <f>SUM(X5:AE5)</f>
+        <v>14</v>
+      </c>
+      <c r="L5" s="23">
+        <f>SUM(AF5:AI5)</f>
+        <v>14</v>
+      </c>
+      <c r="M5" s="24">
+        <f>SUM(AJ5:AN5)</f>
+        <v>14</v>
+      </c>
+      <c r="N5" s="34">
+        <v>14</v>
+      </c>
+      <c r="O5" s="34">
+        <v>14</v>
+      </c>
+      <c r="P5" s="35">
+        <v>-7</v>
+      </c>
+      <c r="Q5" s="33">
+        <v>3</v>
+      </c>
+      <c r="R5" s="41">
+        <v>3</v>
+      </c>
+      <c r="S5" s="33">
+        <v>3</v>
+      </c>
+      <c r="T5" s="41">
+        <v>3</v>
+      </c>
+      <c r="U5" s="33">
+        <v>3</v>
+      </c>
+      <c r="V5" s="33">
+        <v>3</v>
+      </c>
+      <c r="W5" s="33">
+        <v>3</v>
+      </c>
+      <c r="X5" s="35">
+        <v>-7</v>
+      </c>
+      <c r="Y5" s="33">
+        <v>3</v>
+      </c>
+      <c r="Z5" s="33">
+        <v>3</v>
+      </c>
+      <c r="AA5" s="33">
+        <v>3</v>
+      </c>
+      <c r="AB5" s="33">
+        <v>3</v>
+      </c>
+      <c r="AC5" s="33">
+        <v>3</v>
+      </c>
+      <c r="AD5" s="33">
+        <v>3</v>
+      </c>
+      <c r="AE5" s="34">
+        <v>3</v>
+      </c>
+      <c r="AF5" s="37">
+        <v>-1</v>
+      </c>
+      <c r="AG5" s="34">
+        <v>5</v>
+      </c>
+      <c r="AH5" s="34">
+        <v>5</v>
+      </c>
+      <c r="AI5" s="34">
+        <v>5</v>
+      </c>
+      <c r="AJ5" s="37">
+        <v>-6</v>
+      </c>
+      <c r="AK5" s="24">
+        <f>SUM(AO5:AT5)</f>
+        <v>5</v>
+      </c>
+      <c r="AL5" s="34">
+        <v>5</v>
+      </c>
+      <c r="AM5" s="34">
+        <v>5</v>
+      </c>
+      <c r="AN5" s="34">
+        <v>5</v>
+      </c>
+      <c r="AO5" s="37">
+        <v>-5</v>
+      </c>
+      <c r="AP5" s="38">
+        <v>2</v>
+      </c>
+      <c r="AQ5" s="38">
+        <v>2</v>
+      </c>
+      <c r="AR5" s="38">
+        <v>2</v>
+      </c>
+      <c r="AS5" s="38">
+        <v>2</v>
+      </c>
+      <c r="AT5" s="38">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
voorbeelden en kleine debugs
</commit_message>
<xml_diff>
--- a/xls/preparingtables.xlsx
+++ b/xls/preparingtables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="6420" windowWidth="28800" windowHeight="6480" tabRatio="904" activeTab="7"/>
+    <workbookView xWindow="-15" yWindow="6420" windowWidth="28800" windowHeight="6480" tabRatio="904" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="struct_sf16_eng" sheetId="8" r:id="rId1"/>
@@ -20,13 +20,15 @@
     <sheet name="ex3_levelmax" sheetId="26" r:id="rId11"/>
     <sheet name="ex4_outline" sheetId="23" r:id="rId12"/>
     <sheet name="ex5_data" sheetId="34" r:id="rId13"/>
+    <sheet name="ex6_data" sheetId="35" r:id="rId14"/>
+    <sheet name="ex6_outline" sheetId="36" r:id="rId15"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="119">
   <si>
     <t>2d</t>
   </si>
@@ -484,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -555,6 +557,7 @@
     <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1553,8 +1556,8 @@
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1623,7 +1626,7 @@
         <v>2016</v>
       </c>
       <c r="C2" s="17">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D2" s="16">
         <v>80.597999999999999</v>
@@ -1749,7 +1752,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1767,7 +1770,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1775,7 +1778,7 @@
         <v>74</v>
       </c>
       <c r="B3">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1783,7 +1786,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1799,7 +1802,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R38" sqref="R38"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1940,6 +1943,21 @@
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2545,6 +2563,705 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="9" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:AT3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AD3" sqref="AD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="5.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4" style="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" style="32" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" style="24" customWidth="1"/>
+    <col min="13" max="15" width="4" style="24" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4" style="24" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4" style="24" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="4" style="24" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="4" style="24" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="4.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="4" style="24" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="4.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="4" style="24" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4" style="30" bestFit="1" customWidth="1"/>
+    <col min="33" max="35" width="4" style="24" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="4" style="30" bestFit="1" customWidth="1"/>
+    <col min="37" max="40" width="4" style="24" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="5.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="42" max="46" width="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:46" ht="75.75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="25" t="str">
+        <f t="array" ref="E1:AT1">TRANSPOSE(struct_sf16_eng!A2:A44)</f>
+        <v>SCR</v>
+      </c>
+      <c r="F1" s="28" t="str">
+        <v>BSCR</v>
+      </c>
+      <c r="G1" s="22" t="str">
+        <v>operational</v>
+      </c>
+      <c r="H1" s="31" t="str">
+        <v>Adjustment-LACDT</v>
+      </c>
+      <c r="I1" s="29" t="str">
+        <v>BSCR_div</v>
+      </c>
+      <c r="J1" s="22" t="str">
+        <v>market</v>
+      </c>
+      <c r="K1" s="22" t="str">
+        <v>life</v>
+      </c>
+      <c r="L1" s="22" t="str">
+        <v>nonlife</v>
+      </c>
+      <c r="M1" s="22" t="str">
+        <v>health</v>
+      </c>
+      <c r="N1" s="22" t="str">
+        <v>cp-default</v>
+      </c>
+      <c r="O1" s="22" t="str">
+        <v>intangibles</v>
+      </c>
+      <c r="P1" s="29" t="str">
+        <v>market_div</v>
+      </c>
+      <c r="Q1" s="22" t="str">
+        <v>m_interestrate</v>
+      </c>
+      <c r="R1" s="22" t="str">
+        <v>m_equity</v>
+      </c>
+      <c r="S1" s="22" t="str">
+        <v>m_property</v>
+      </c>
+      <c r="T1" s="22" t="str">
+        <v>m_spread</v>
+      </c>
+      <c r="U1" s="22" t="str">
+        <v>m_currency</v>
+      </c>
+      <c r="V1" s="22" t="str">
+        <v>m_concentration</v>
+      </c>
+      <c r="W1" s="22" t="str">
+        <v>m_illiquidity</v>
+      </c>
+      <c r="X1" s="29" t="str">
+        <v>life_div</v>
+      </c>
+      <c r="Y1" s="22" t="str">
+        <v>l_mortality</v>
+      </c>
+      <c r="Z1" s="22" t="str">
+        <v>l_longevity</v>
+      </c>
+      <c r="AA1" s="22" t="str">
+        <v>l_disability</v>
+      </c>
+      <c r="AB1" s="22" t="str">
+        <v>l_lapse</v>
+      </c>
+      <c r="AC1" s="22" t="str">
+        <v>l_expenses</v>
+      </c>
+      <c r="AD1" s="22" t="str">
+        <v>l_revision</v>
+      </c>
+      <c r="AE1" s="22" t="str">
+        <v>l_CAT</v>
+      </c>
+      <c r="AF1" s="29" t="str">
+        <v>nonlife_div</v>
+      </c>
+      <c r="AG1" s="22" t="str">
+        <v>n_premiumreserve</v>
+      </c>
+      <c r="AH1" s="22" t="str">
+        <v>n_lapse</v>
+      </c>
+      <c r="AI1" s="22" t="str">
+        <v>n_CAT</v>
+      </c>
+      <c r="AJ1" s="29" t="str">
+        <v>health_div</v>
+      </c>
+      <c r="AK1" s="22" t="str">
+        <v>h_SLT</v>
+      </c>
+      <c r="AL1" s="22" t="str">
+        <v>h_CAT</v>
+      </c>
+      <c r="AM1" s="22" t="str">
+        <v>h_n_premiumres</v>
+      </c>
+      <c r="AN1" s="22" t="str">
+        <v>h_n_lapse</v>
+      </c>
+      <c r="AO1" s="29" t="str">
+        <v>h_SLT_div</v>
+      </c>
+      <c r="AP1" s="8" t="str">
+        <v>h_s_mortality</v>
+      </c>
+      <c r="AQ1" s="8" t="str">
+        <v>h_s_longevity</v>
+      </c>
+      <c r="AR1" s="8" t="str">
+        <v>h_s_disability</v>
+      </c>
+      <c r="AS1" s="8" t="str">
+        <v>h_s_lapse</v>
+      </c>
+      <c r="AT1" s="8" t="str">
+        <v>h_s_expenses</v>
+      </c>
+    </row>
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="26">
+        <f>SUM(F2:H2)</f>
+        <v>80</v>
+      </c>
+      <c r="F2" s="26">
+        <f>SUM(I2:O2)</f>
+        <v>75</v>
+      </c>
+      <c r="G2" s="34">
+        <v>25</v>
+      </c>
+      <c r="H2" s="40">
+        <v>-20</v>
+      </c>
+      <c r="I2" s="37">
+        <v>-9</v>
+      </c>
+      <c r="J2" s="23">
+        <f>SUM(P2:W2)</f>
+        <v>14</v>
+      </c>
+      <c r="K2" s="23">
+        <f>SUM(X2:AE2)</f>
+        <v>14</v>
+      </c>
+      <c r="L2" s="23">
+        <f>SUM(AF2:AI2)</f>
+        <v>14</v>
+      </c>
+      <c r="M2" s="24">
+        <f>SUM(AJ2:AN2)</f>
+        <v>14</v>
+      </c>
+      <c r="N2" s="34">
+        <v>14</v>
+      </c>
+      <c r="O2" s="34">
+        <v>14</v>
+      </c>
+      <c r="P2" s="35">
+        <v>-7</v>
+      </c>
+      <c r="Q2" s="33">
+        <v>3</v>
+      </c>
+      <c r="R2" s="41">
+        <v>3</v>
+      </c>
+      <c r="S2" s="33">
+        <v>3</v>
+      </c>
+      <c r="T2" s="41">
+        <v>3</v>
+      </c>
+      <c r="U2" s="33">
+        <v>3</v>
+      </c>
+      <c r="V2" s="33">
+        <v>3</v>
+      </c>
+      <c r="W2" s="33">
+        <v>3</v>
+      </c>
+      <c r="X2" s="35">
+        <v>-7</v>
+      </c>
+      <c r="Y2" s="33">
+        <v>3</v>
+      </c>
+      <c r="Z2" s="33">
+        <v>3</v>
+      </c>
+      <c r="AA2" s="33">
+        <v>3</v>
+      </c>
+      <c r="AB2" s="33">
+        <v>3</v>
+      </c>
+      <c r="AC2" s="33">
+        <v>3</v>
+      </c>
+      <c r="AD2" s="33">
+        <v>3</v>
+      </c>
+      <c r="AE2" s="34">
+        <v>3</v>
+      </c>
+      <c r="AF2" s="37">
+        <v>-1</v>
+      </c>
+      <c r="AG2" s="34">
+        <v>5</v>
+      </c>
+      <c r="AH2" s="34">
+        <v>5</v>
+      </c>
+      <c r="AI2" s="34">
+        <v>5</v>
+      </c>
+      <c r="AJ2" s="37">
+        <v>-6</v>
+      </c>
+      <c r="AK2" s="24">
+        <f>SUM(AO2:AT2)</f>
+        <v>5</v>
+      </c>
+      <c r="AL2" s="34">
+        <v>5</v>
+      </c>
+      <c r="AM2" s="34">
+        <v>5</v>
+      </c>
+      <c r="AN2" s="34">
+        <v>5</v>
+      </c>
+      <c r="AO2" s="37">
+        <v>-2.5</v>
+      </c>
+      <c r="AP2" s="38">
+        <v>1.5</v>
+      </c>
+      <c r="AQ2" s="38">
+        <v>1.5</v>
+      </c>
+      <c r="AR2" s="38">
+        <v>1.5</v>
+      </c>
+      <c r="AS2" s="38">
+        <v>1.5</v>
+      </c>
+      <c r="AT2" s="38">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="26">
+        <f>SUM(F3:H3)</f>
+        <v>75</v>
+      </c>
+      <c r="F3" s="26">
+        <f>SUM(I3:O3)</f>
+        <v>68</v>
+      </c>
+      <c r="G3" s="34">
+        <v>20</v>
+      </c>
+      <c r="H3" s="40">
+        <v>-13</v>
+      </c>
+      <c r="I3" s="37">
+        <v>-6</v>
+      </c>
+      <c r="J3" s="23">
+        <f>SUM(P3:W3)</f>
+        <v>12.5</v>
+      </c>
+      <c r="K3" s="23">
+        <f>SUM(X3:AE3)</f>
+        <v>11</v>
+      </c>
+      <c r="L3" s="23">
+        <f>SUM(AF3:AI3)</f>
+        <v>13.5</v>
+      </c>
+      <c r="M3" s="24">
+        <f>SUM(AJ3:AN3)</f>
+        <v>13</v>
+      </c>
+      <c r="N3" s="34">
+        <v>12</v>
+      </c>
+      <c r="O3" s="34">
+        <v>12</v>
+      </c>
+      <c r="P3" s="35">
+        <v>-3.25</v>
+      </c>
+      <c r="Q3" s="33">
+        <v>2.25</v>
+      </c>
+      <c r="R3" s="41">
+        <v>2.25</v>
+      </c>
+      <c r="S3" s="33">
+        <v>2.25</v>
+      </c>
+      <c r="T3" s="41">
+        <v>2.25</v>
+      </c>
+      <c r="U3" s="33">
+        <v>2.25</v>
+      </c>
+      <c r="V3" s="33">
+        <v>2.25</v>
+      </c>
+      <c r="W3" s="33">
+        <v>2.25</v>
+      </c>
+      <c r="X3" s="35">
+        <v>-6.5</v>
+      </c>
+      <c r="Y3" s="33">
+        <v>1.5</v>
+      </c>
+      <c r="Z3" s="33">
+        <v>2</v>
+      </c>
+      <c r="AA3" s="33">
+        <v>2.5</v>
+      </c>
+      <c r="AB3" s="33">
+        <v>3.5</v>
+      </c>
+      <c r="AC3" s="33">
+        <v>3</v>
+      </c>
+      <c r="AD3" s="33">
+        <v>2.5</v>
+      </c>
+      <c r="AE3" s="34">
+        <v>2.5</v>
+      </c>
+      <c r="AF3" s="37">
+        <v>-1.5</v>
+      </c>
+      <c r="AG3" s="34">
+        <v>4</v>
+      </c>
+      <c r="AH3" s="34">
+        <v>5</v>
+      </c>
+      <c r="AI3" s="34">
+        <v>6</v>
+      </c>
+      <c r="AJ3" s="37">
+        <v>-3</v>
+      </c>
+      <c r="AK3" s="24">
+        <f>SUM(AO3:AT3)</f>
+        <v>4</v>
+      </c>
+      <c r="AL3" s="34">
+        <v>4</v>
+      </c>
+      <c r="AM3" s="34">
+        <v>4</v>
+      </c>
+      <c r="AN3" s="34">
+        <v>4</v>
+      </c>
+      <c r="AO3" s="42">
+        <v>-2.25</v>
+      </c>
+      <c r="AP3" s="38">
+        <v>1.25</v>
+      </c>
+      <c r="AQ3" s="38">
+        <v>1.25</v>
+      </c>
+      <c r="AR3" s="38">
+        <v>1.25</v>
+      </c>
+      <c r="AS3" s="38">
+        <v>1.25</v>
+      </c>
+      <c r="AT3" s="38">
+        <v>1.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="9" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
@@ -2552,7 +3269,7 @@
   </sheetPr>
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -3240,7 +3957,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3381,6 +4098,21 @@
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -3468,7 +4200,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3609,6 +4341,21 @@
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -4080,8 +4827,8 @@
   </sheetPr>
   <dimension ref="A1:AT5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4264,9 +5011,11 @@
       <c r="A2" s="17">
         <v>1</v>
       </c>
-      <c r="B2" s="17"/>
+      <c r="B2" s="17">
+        <v>2</v>
+      </c>
       <c r="C2" s="17">
-        <v>2017</v>
+        <v>2021</v>
       </c>
       <c r="D2" s="17">
         <v>230</v>
@@ -4409,11 +5158,9 @@
       <c r="A3" s="17">
         <v>2</v>
       </c>
-      <c r="B3" s="17">
-        <v>1</v>
-      </c>
+      <c r="B3" s="17"/>
       <c r="C3" s="17">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="D3" s="17">
         <v>234</v>
@@ -4427,7 +5174,7 @@
         <v>103.85622317596567</v>
       </c>
       <c r="G3" s="33">
-        <f t="shared" ref="F3:AD5" si="0">85/$E$2*G2</f>
+        <f t="shared" ref="G3:AD4" si="0">85/$E$2*G2</f>
         <v>4.2560801144492126</v>
       </c>
       <c r="H3" s="39">
@@ -4576,7 +5323,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>2021</v>
@@ -4732,148 +5479,46 @@
       </c>
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>2023</v>
-      </c>
-      <c r="D5">
-        <v>228</v>
-      </c>
-      <c r="E5" s="26">
-        <f>SUM(F5:H5)</f>
-        <v>80</v>
-      </c>
-      <c r="F5" s="26">
-        <f>SUM(I5:O5)</f>
-        <v>75</v>
-      </c>
-      <c r="G5" s="34">
-        <v>25</v>
-      </c>
-      <c r="H5" s="40">
-        <v>-20</v>
-      </c>
-      <c r="I5" s="37">
-        <v>-9</v>
-      </c>
-      <c r="J5" s="23">
-        <f>SUM(P5:W5)</f>
-        <v>14</v>
-      </c>
-      <c r="K5" s="23">
-        <f>SUM(X5:AE5)</f>
-        <v>14</v>
-      </c>
-      <c r="L5" s="23">
-        <f>SUM(AF5:AI5)</f>
-        <v>14</v>
-      </c>
-      <c r="M5" s="24">
-        <f>SUM(AJ5:AN5)</f>
-        <v>14</v>
-      </c>
-      <c r="N5" s="34">
-        <v>14</v>
-      </c>
-      <c r="O5" s="34">
-        <v>14</v>
-      </c>
-      <c r="P5" s="35">
-        <v>-7</v>
-      </c>
-      <c r="Q5" s="33">
-        <v>3</v>
-      </c>
-      <c r="R5" s="41">
-        <v>3</v>
-      </c>
-      <c r="S5" s="33">
-        <v>3</v>
-      </c>
-      <c r="T5" s="41">
-        <v>3</v>
-      </c>
-      <c r="U5" s="33">
-        <v>3</v>
-      </c>
-      <c r="V5" s="33">
-        <v>3</v>
-      </c>
-      <c r="W5" s="33">
-        <v>3</v>
-      </c>
-      <c r="X5" s="35">
-        <v>-7</v>
-      </c>
-      <c r="Y5" s="33">
-        <v>3</v>
-      </c>
-      <c r="Z5" s="33">
-        <v>3</v>
-      </c>
-      <c r="AA5" s="33">
-        <v>3</v>
-      </c>
-      <c r="AB5" s="33">
-        <v>3</v>
-      </c>
-      <c r="AC5" s="33">
-        <v>3</v>
-      </c>
-      <c r="AD5" s="33">
-        <v>3</v>
-      </c>
-      <c r="AE5" s="34">
-        <v>3</v>
-      </c>
-      <c r="AF5" s="37">
-        <v>-1</v>
-      </c>
-      <c r="AG5" s="34">
-        <v>5</v>
-      </c>
-      <c r="AH5" s="34">
-        <v>5</v>
-      </c>
-      <c r="AI5" s="34">
-        <v>5</v>
-      </c>
-      <c r="AJ5" s="37">
-        <v>-6</v>
-      </c>
-      <c r="AK5" s="24">
-        <f>SUM(AO5:AT5)</f>
-        <v>5</v>
-      </c>
-      <c r="AL5" s="34">
-        <v>5</v>
-      </c>
-      <c r="AM5" s="34">
-        <v>5</v>
-      </c>
-      <c r="AN5" s="34">
-        <v>5</v>
-      </c>
-      <c r="AO5" s="37">
-        <v>-5</v>
-      </c>
-      <c r="AP5" s="38">
-        <v>2</v>
-      </c>
-      <c r="AQ5" s="38">
-        <v>2</v>
-      </c>
-      <c r="AR5" s="38">
-        <v>2</v>
-      </c>
-      <c r="AS5" s="38">
-        <v>2</v>
-      </c>
-      <c r="AT5" s="38">
-        <v>2</v>
-      </c>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="35"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="41"/>
+      <c r="S5" s="33"/>
+      <c r="T5" s="41"/>
+      <c r="U5" s="33"/>
+      <c r="V5" s="33"/>
+      <c r="W5" s="33"/>
+      <c r="X5" s="35"/>
+      <c r="Y5" s="33"/>
+      <c r="Z5" s="33"/>
+      <c r="AA5" s="33"/>
+      <c r="AB5" s="33"/>
+      <c r="AC5" s="33"/>
+      <c r="AD5" s="33"/>
+      <c r="AE5" s="34"/>
+      <c r="AF5" s="37"/>
+      <c r="AG5" s="34"/>
+      <c r="AH5" s="34"/>
+      <c r="AI5" s="34"/>
+      <c r="AJ5" s="37"/>
+      <c r="AL5" s="34"/>
+      <c r="AM5" s="34"/>
+      <c r="AN5" s="34"/>
+      <c r="AO5" s="37"/>
+      <c r="AP5" s="38"/>
+      <c r="AQ5" s="38"/>
+      <c r="AR5" s="38"/>
+      <c r="AS5" s="38"/>
+      <c r="AT5" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
einde dag, example6 werkend
</commit_message>
<xml_diff>
--- a/xls/preparingtables.xlsx
+++ b/xls/preparingtables.xlsx
@@ -19,7 +19,7 @@
     <sheet name="ex4_levelmax" sheetId="26" r:id="rId10"/>
     <sheet name="ex5_data_redundant" sheetId="34" r:id="rId11"/>
     <sheet name="ex5_plotdetails_redundant" sheetId="46" r:id="rId12"/>
-    <sheet name="ex6_struct" sheetId="38" r:id="rId13"/>
+    <sheet name="ex6_struct_and_colors" sheetId="38" r:id="rId13"/>
     <sheet name="ex6_data" sheetId="39" r:id="rId14"/>
     <sheet name="ex6_data_adapted" sheetId="42" r:id="rId15"/>
     <sheet name="ex6_levelmax" sheetId="40" r:id="rId16"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1256" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="264">
   <si>
     <t>2d</t>
   </si>
@@ -701,6 +701,129 @@
   </si>
   <si>
     <t>nonlife_other</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>006d2c</t>
+  </si>
+  <si>
+    <t>66c2a4</t>
+  </si>
+  <si>
+    <t>fee8c8</t>
+  </si>
+  <si>
+    <t>fff7ec</t>
+  </si>
+  <si>
+    <t>2ca25f</t>
+  </si>
+  <si>
+    <t>b2e2e2</t>
+  </si>
+  <si>
+    <t>edf8fb</t>
+  </si>
+  <si>
+    <t>morb_uncertainty</t>
+  </si>
+  <si>
+    <t>morb_volatility</t>
+  </si>
+  <si>
+    <t>morb_prior</t>
+  </si>
+  <si>
+    <t>morb_calamity</t>
+  </si>
+  <si>
+    <t>expense_level</t>
+  </si>
+  <si>
+    <t>expense_inflation</t>
+  </si>
+  <si>
+    <t>2b8cbe</t>
+  </si>
+  <si>
+    <t>74a9cf</t>
+  </si>
+  <si>
+    <t>bdc9e1</t>
+  </si>
+  <si>
+    <t>f1eef6</t>
+  </si>
+  <si>
+    <t>045a8d</t>
+  </si>
+  <si>
+    <t>8856a7</t>
+  </si>
+  <si>
+    <t>8c96c6</t>
+  </si>
+  <si>
+    <t>b3cde3</t>
+  </si>
+  <si>
+    <t>810f7c</t>
+  </si>
+  <si>
+    <t>4b4b4b</t>
+  </si>
+  <si>
+    <t>7d7d7d</t>
+  </si>
+  <si>
+    <t>aeaeae</t>
+  </si>
+  <si>
+    <t>c8c8c8</t>
+  </si>
+  <si>
+    <t>e1e1e1</t>
+  </si>
+  <si>
+    <t>ffffff</t>
+  </si>
+  <si>
+    <t>191919</t>
+  </si>
+  <si>
+    <t>323232</t>
+  </si>
+  <si>
+    <t>646464</t>
+  </si>
+  <si>
+    <t>969696</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>800026</t>
+  </si>
+  <si>
+    <t>bd0026</t>
+  </si>
+  <si>
+    <t>e31a1c</t>
+  </si>
+  <si>
+    <t>fc4e2a</t>
+  </si>
+  <si>
+    <t>fd8d3c</t>
+  </si>
+  <si>
+    <t>ffeda0</t>
+  </si>
+  <si>
+    <t>feb24c</t>
   </si>
 </sst>
 </file>
@@ -761,7 +884,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -777,6 +900,96 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -829,7 +1042,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -948,6 +1161,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1260,8 +1490,8 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="20" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G45" sqref="G45"/>
+      <pane ySplit="20" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3586,10 +3816,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:O55"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3597,10 +3827,9 @@
     <col min="1" max="2" width="21.28515625" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>205</v>
       </c>
@@ -3625,20 +3854,8 @@
       <c r="H1" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="L1" t="s">
-        <v>212</v>
-      </c>
-      <c r="M1" t="s">
-        <v>213</v>
-      </c>
-      <c r="N1" t="s">
-        <v>168</v>
-      </c>
-      <c r="O1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -3653,20 +3870,14 @@
         <f>A2</f>
         <v>SCR</v>
       </c>
-      <c r="L2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" t="s">
-        <v>74</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="G2" t="s">
         <v>170</v>
       </c>
-      <c r="O2" t="s">
+      <c r="H2" s="13" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -3680,20 +3891,15 @@
         <f t="shared" ref="E3:E50" si="0">A3</f>
         <v>BSCR</v>
       </c>
-      <c r="L3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M3" t="s">
-        <v>113</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="G3" t="s">
         <v>172</v>
       </c>
-      <c r="O3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H3" t="str">
+        <f>VLOOKUP(C3,$D$2:$G$55,4,FALSE)</f>
+        <v>1f78b4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -3705,20 +3911,15 @@
         <f t="shared" si="0"/>
         <v>operational</v>
       </c>
-      <c r="L4" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" t="s">
-        <v>75</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="G4" t="s">
         <v>173</v>
       </c>
-      <c r="O4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H4" t="str">
+        <f>VLOOKUP(C4,$D$2:$G$55,4,FALSE)</f>
+        <v>1f78b4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>32</v>
       </c>
@@ -3731,14 +3932,8 @@
         <f t="shared" si="0"/>
         <v>Adjustment-LACDT</v>
       </c>
-      <c r="L5" t="s">
-        <v>32</v>
-      </c>
-      <c r="M5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -3750,14 +3945,8 @@
         <f t="shared" si="0"/>
         <v>BSCR_div</v>
       </c>
-      <c r="L6" t="s">
-        <v>30</v>
-      </c>
-      <c r="M6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>158</v>
       </c>
@@ -3771,20 +3960,18 @@
         <f t="shared" si="0"/>
         <v>MBC</v>
       </c>
-      <c r="L7" t="s">
-        <v>12</v>
-      </c>
-      <c r="M7" t="s">
-        <v>78</v>
-      </c>
-      <c r="N7" t="s">
-        <v>174</v>
-      </c>
-      <c r="O7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>256</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="H7" t="str">
+        <f>VLOOKUP(C7,$D$2:$G$55,4,FALSE)</f>
+        <v>48b0eb</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>157</v>
       </c>
@@ -3799,20 +3986,18 @@
         <f t="shared" si="0"/>
         <v>insurance</v>
       </c>
-      <c r="L8" t="s">
-        <v>14</v>
-      </c>
-      <c r="M8" t="s">
-        <v>79</v>
-      </c>
-      <c r="N8" t="s">
-        <v>176</v>
-      </c>
-      <c r="O8" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>256</v>
+      </c>
+      <c r="G8" t="s">
+        <v>258</v>
+      </c>
+      <c r="H8" t="str">
+        <f>VLOOKUP(C8,$D$2:$G$55,4,FALSE)</f>
+        <v>48b0eb</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>156</v>
       </c>
@@ -3823,20 +4008,8 @@
         <f t="shared" si="0"/>
         <v>MBC_div</v>
       </c>
-      <c r="L9" t="s">
-        <v>214</v>
-      </c>
-      <c r="M9" t="s">
-        <v>80</v>
-      </c>
-      <c r="N9" t="s">
-        <v>177</v>
-      </c>
-      <c r="O9" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>154</v>
       </c>
@@ -3850,20 +4023,18 @@
         <f t="shared" si="0"/>
         <v>MC</v>
       </c>
-      <c r="L10" t="s">
-        <v>33</v>
-      </c>
-      <c r="M10" t="s">
-        <v>101</v>
-      </c>
-      <c r="N10" t="s">
-        <v>175</v>
-      </c>
-      <c r="O10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>256</v>
+      </c>
+      <c r="G10" t="s">
+        <v>259</v>
+      </c>
+      <c r="H10" t="str">
+        <f>VLOOKUP(C10,$D$2:$G$55,4,FALSE)</f>
+        <v>800026</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>153</v>
       </c>
@@ -3876,20 +4047,18 @@
         <f t="shared" si="0"/>
         <v>basis</v>
       </c>
-      <c r="L11" t="s">
-        <v>31</v>
-      </c>
-      <c r="M11" t="s">
-        <v>81</v>
-      </c>
-      <c r="N11" t="s">
-        <v>178</v>
-      </c>
-      <c r="O11" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>256</v>
+      </c>
+      <c r="G11" t="s">
+        <v>260</v>
+      </c>
+      <c r="H11" t="str">
+        <f>VLOOKUP(C11,$D$2:$G$55,4,FALSE)</f>
+        <v>800026</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>152</v>
       </c>
@@ -3902,20 +4071,8 @@
         <f t="shared" si="0"/>
         <v>MC_div</v>
       </c>
-      <c r="L12" t="s">
-        <v>65</v>
-      </c>
-      <c r="M12" t="s">
-        <v>65</v>
-      </c>
-      <c r="N12" t="s">
-        <v>179</v>
-      </c>
-      <c r="O12" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -3929,14 +4086,15 @@
         <f t="shared" si="0"/>
         <v>market</v>
       </c>
-      <c r="L13" t="s">
-        <v>10</v>
-      </c>
-      <c r="M13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>251</v>
+      </c>
+      <c r="H13" t="str">
+        <f>VLOOKUP(C13,$D$2:$G$55,4,FALSE)</f>
+        <v>e31a1c</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>151</v>
       </c>
@@ -3950,20 +4108,15 @@
         <f t="shared" si="0"/>
         <v>counterpartydefault</v>
       </c>
-      <c r="L14" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="M14" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="N14" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="O14" s="22" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="H14" t="str">
+        <f>VLOOKUP(C14,$D$2:$G$55,4,FALSE)</f>
+        <v>e31a1c</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>10</v>
       </c>
@@ -3975,20 +4128,8 @@
         <f t="shared" si="0"/>
         <v>market_div</v>
       </c>
-      <c r="L15" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="M15" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="N15" s="22" t="s">
-        <v>181</v>
-      </c>
-      <c r="O15" s="22" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>150</v>
       </c>
@@ -3999,20 +4140,15 @@
         <f t="shared" si="0"/>
         <v>equity</v>
       </c>
-      <c r="L16" t="s">
-        <v>51</v>
-      </c>
-      <c r="M16" t="s">
-        <v>85</v>
-      </c>
-      <c r="N16" t="s">
-        <v>182</v>
-      </c>
-      <c r="O16" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G16" s="87" t="s">
+        <v>252</v>
+      </c>
+      <c r="H16" t="str">
+        <f>VLOOKUP(C16,$D$2:$G$55,4,FALSE)</f>
+        <v>ffffff</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>149</v>
       </c>
@@ -4023,20 +4159,15 @@
         <f t="shared" si="0"/>
         <v>interest</v>
       </c>
-      <c r="L17" t="s">
-        <v>52</v>
-      </c>
-      <c r="M17" t="s">
-        <v>52</v>
-      </c>
-      <c r="N17" t="s">
-        <v>183</v>
-      </c>
-      <c r="O17" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G17" s="85" t="s">
+        <v>253</v>
+      </c>
+      <c r="H17" t="str">
+        <f>VLOOKUP(C17,$D$2:$G$55,4,FALSE)</f>
+        <v>ffffff</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>148</v>
       </c>
@@ -4047,20 +4178,15 @@
         <f t="shared" si="0"/>
         <v>creditspread</v>
       </c>
-      <c r="L18" t="s">
-        <v>53</v>
-      </c>
-      <c r="M18" t="s">
-        <v>86</v>
-      </c>
-      <c r="N18" t="s">
-        <v>184</v>
-      </c>
-      <c r="O18" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G18" s="85" t="s">
+        <v>246</v>
+      </c>
+      <c r="H18" t="str">
+        <f>VLOOKUP(C18,$D$2:$G$55,4,FALSE)</f>
+        <v>ffffff</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>147</v>
       </c>
@@ -4071,20 +4197,15 @@
         <f t="shared" si="0"/>
         <v>realestate</v>
       </c>
-      <c r="L19" t="s">
-        <v>54</v>
-      </c>
-      <c r="M19" t="s">
-        <v>87</v>
-      </c>
-      <c r="N19" t="s">
-        <v>185</v>
-      </c>
-      <c r="O19" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G19" s="85" t="s">
+        <v>254</v>
+      </c>
+      <c r="H19" t="str">
+        <f>VLOOKUP(C19,$D$2:$G$55,4,FALSE)</f>
+        <v>ffffff</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>146</v>
       </c>
@@ -4095,20 +4216,15 @@
         <f t="shared" si="0"/>
         <v>inflation</v>
       </c>
-      <c r="L20" t="s">
-        <v>73</v>
-      </c>
-      <c r="M20" t="s">
-        <v>88</v>
-      </c>
-      <c r="N20" t="s">
-        <v>186</v>
-      </c>
-      <c r="O20" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G20" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="H20" t="str">
+        <f>VLOOKUP(C20,$D$2:$G$55,4,FALSE)</f>
+        <v>ffffff</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>145</v>
       </c>
@@ -4119,14 +4235,15 @@
         <f t="shared" si="0"/>
         <v>equity_impliedvol</v>
       </c>
-      <c r="L21" t="s">
-        <v>7</v>
-      </c>
-      <c r="M21" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G21" s="86" t="s">
+        <v>255</v>
+      </c>
+      <c r="H21" t="str">
+        <f>VLOOKUP(C21,$D$2:$G$55,4,FALSE)</f>
+        <v>ffffff</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>144</v>
       </c>
@@ -4137,20 +4254,15 @@
         <f t="shared" si="0"/>
         <v>interest_impliedvol</v>
       </c>
-      <c r="L22" t="s">
-        <v>36</v>
-      </c>
-      <c r="M22" t="s">
-        <v>90</v>
-      </c>
-      <c r="N22" t="s">
-        <v>187</v>
-      </c>
-      <c r="O22" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G22" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="H22" t="str">
+        <f>VLOOKUP(C22,$D$2:$G$55,4,FALSE)</f>
+        <v>ffffff</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>143</v>
       </c>
@@ -4161,20 +4273,15 @@
         <f t="shared" si="0"/>
         <v>FX</v>
       </c>
-      <c r="L23" t="s">
-        <v>37</v>
-      </c>
-      <c r="M23" t="s">
-        <v>91</v>
-      </c>
-      <c r="N23" t="s">
-        <v>188</v>
-      </c>
-      <c r="O23" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G23" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="H23" t="str">
+        <f>VLOOKUP(C23,$D$2:$G$55,4,FALSE)</f>
+        <v>ffffff</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>142</v>
       </c>
@@ -4185,20 +4292,15 @@
         <f t="shared" si="0"/>
         <v>FX_impliedvol</v>
       </c>
-      <c r="L24" t="s">
-        <v>38</v>
-      </c>
-      <c r="M24" t="s">
-        <v>92</v>
-      </c>
-      <c r="N24" t="s">
-        <v>189</v>
-      </c>
-      <c r="O24" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G24" s="88" t="s">
+        <v>250</v>
+      </c>
+      <c r="H24" t="str">
+        <f>VLOOKUP(C24,$D$2:$G$55,4,FALSE)</f>
+        <v>ffffff</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>141</v>
       </c>
@@ -4209,20 +4311,18 @@
         <f t="shared" si="0"/>
         <v>type1</v>
       </c>
-      <c r="L25" t="s">
-        <v>39</v>
-      </c>
-      <c r="M25" t="s">
-        <v>93</v>
-      </c>
-      <c r="N25" t="s">
-        <v>190</v>
-      </c>
-      <c r="O25" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>256</v>
+      </c>
+      <c r="G25" t="s">
+        <v>261</v>
+      </c>
+      <c r="H25" t="str">
+        <f>VLOOKUP(C25,$D$2:$G$55,4,FALSE)</f>
+        <v>ffeda0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>140</v>
       </c>
@@ -4233,20 +4333,18 @@
         <f t="shared" si="0"/>
         <v>type2</v>
       </c>
-      <c r="L26" t="s">
-        <v>40</v>
-      </c>
-      <c r="M26" t="s">
-        <v>94</v>
-      </c>
-      <c r="N26" t="s">
-        <v>191</v>
-      </c>
-      <c r="O26" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>256</v>
+      </c>
+      <c r="G26" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="H26" t="str">
+        <f>VLOOKUP(C26,$D$2:$G$55,4,FALSE)</f>
+        <v>ffeda0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -4257,20 +4355,9 @@
         <f t="shared" si="0"/>
         <v>insurance_div</v>
       </c>
-      <c r="L27" t="s">
-        <v>41</v>
-      </c>
-      <c r="M27" t="s">
-        <v>95</v>
-      </c>
-      <c r="N27" t="s">
-        <v>192</v>
-      </c>
-      <c r="O27" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G27" s="22"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>137</v>
       </c>
@@ -4284,20 +4371,16 @@
         <f t="shared" si="0"/>
         <v>business</v>
       </c>
-      <c r="L28" t="s">
-        <v>42</v>
-      </c>
-      <c r="M28" t="s">
-        <v>42</v>
-      </c>
-      <c r="N28" t="s">
-        <v>193</v>
-      </c>
-      <c r="O28" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F28" s="13"/>
+      <c r="G28" s="74" t="s">
+        <v>180</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" ref="H28:H50" si="1">VLOOKUP(C28,$D$2:$G$55,4,FALSE)</f>
+        <v>bd0026</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -4311,14 +4394,15 @@
         <f t="shared" si="0"/>
         <v>life</v>
       </c>
-      <c r="L29" t="s">
-        <v>5</v>
-      </c>
-      <c r="M29" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G29" s="73" t="s">
+        <v>224</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="1"/>
+        <v>bd0026</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>136</v>
       </c>
@@ -4332,20 +4416,15 @@
         <f t="shared" si="0"/>
         <v>morbidity</v>
       </c>
-      <c r="L30" t="s">
-        <v>43</v>
-      </c>
-      <c r="M30" t="s">
-        <v>97</v>
-      </c>
-      <c r="N30" t="s">
-        <v>171</v>
-      </c>
-      <c r="O30" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G30" s="78" t="s">
+        <v>241</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="1"/>
+        <v>bd0026</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -4359,62 +4438,53 @@
         <f t="shared" si="0"/>
         <v>nonlife</v>
       </c>
-      <c r="L31" t="s">
-        <v>44</v>
-      </c>
-      <c r="M31" t="s">
-        <v>98</v>
-      </c>
-      <c r="N31" t="s">
-        <v>194</v>
-      </c>
-      <c r="O31" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G31" s="77" t="s">
+        <v>245</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="1"/>
+        <v>bd0026</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>135</v>
+        <v>235</v>
       </c>
       <c r="C32" t="s">
         <v>35</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="0"/>
-        <v>expense level</v>
-      </c>
-      <c r="L32" t="s">
-        <v>45</v>
-      </c>
-      <c r="M32" t="s">
-        <v>99</v>
-      </c>
-      <c r="N32" t="s">
-        <v>195</v>
-      </c>
-      <c r="O32" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+        <v>expense_level</v>
+      </c>
+      <c r="G32" s="79" t="s">
+        <v>181</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="1"/>
+        <v>990000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>134</v>
+        <v>236</v>
       </c>
       <c r="C33" t="s">
         <v>35</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="0"/>
-        <v>expense inflation</v>
-      </c>
-      <c r="L33" t="s">
-        <v>63</v>
-      </c>
-      <c r="M33" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+        <v>expense_inflation</v>
+      </c>
+      <c r="G33" t="s">
+        <v>182</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="1"/>
+        <v>990000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>133</v>
       </c>
@@ -4425,20 +4495,15 @@
         <f t="shared" si="0"/>
         <v>continuation</v>
       </c>
-      <c r="L34" t="s">
-        <v>46</v>
-      </c>
-      <c r="M34" t="s">
-        <v>102</v>
-      </c>
-      <c r="N34" t="s">
-        <v>196</v>
-      </c>
-      <c r="O34" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>183</v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="1"/>
+        <v>990000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>132</v>
       </c>
@@ -4449,20 +4514,15 @@
         <f t="shared" si="0"/>
         <v>persistency_uncertain</v>
       </c>
-      <c r="L35" t="s">
-        <v>47</v>
-      </c>
-      <c r="M35" t="s">
-        <v>103</v>
-      </c>
-      <c r="N35" t="s">
-        <v>197</v>
-      </c>
-      <c r="O35" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>184</v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="1"/>
+        <v>990000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>131</v>
       </c>
@@ -4473,20 +4533,15 @@
         <f t="shared" si="0"/>
         <v>persistency_volatility</v>
       </c>
-      <c r="L36" t="s">
-        <v>56</v>
-      </c>
-      <c r="M36" t="s">
-        <v>104</v>
-      </c>
-      <c r="N36" t="s">
-        <v>198</v>
-      </c>
-      <c r="O36" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>185</v>
+      </c>
+      <c r="H36" t="str">
+        <f t="shared" si="1"/>
+        <v>990000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>130</v>
       </c>
@@ -4497,20 +4552,15 @@
         <f t="shared" si="0"/>
         <v>persistency_calamity</v>
       </c>
-      <c r="L37" t="s">
-        <v>55</v>
-      </c>
-      <c r="M37" t="s">
-        <v>105</v>
-      </c>
-      <c r="N37" t="s">
-        <v>199</v>
-      </c>
-      <c r="O37" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>226</v>
+      </c>
+      <c r="H37" t="str">
+        <f t="shared" si="1"/>
+        <v>990000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>129</v>
       </c>
@@ -4521,14 +4571,15 @@
         <f t="shared" si="0"/>
         <v>premium_rerating</v>
       </c>
-      <c r="L38" t="s">
-        <v>48</v>
-      </c>
-      <c r="M38" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G38" s="76" t="s">
+        <v>227</v>
+      </c>
+      <c r="H38" t="str">
+        <f t="shared" si="1"/>
+        <v>990000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>128</v>
       </c>
@@ -4539,20 +4590,15 @@
         <f t="shared" si="0"/>
         <v>mortality_trend</v>
       </c>
-      <c r="L39" t="s">
-        <v>57</v>
-      </c>
-      <c r="M39" t="s">
-        <v>107</v>
-      </c>
-      <c r="N39" t="s">
-        <v>200</v>
-      </c>
-      <c r="O39" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G39" s="81" t="s">
+        <v>228</v>
+      </c>
+      <c r="H39" t="str">
+        <f t="shared" si="1"/>
+        <v>006d2c</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>127</v>
       </c>
@@ -4563,20 +4609,15 @@
         <f t="shared" si="0"/>
         <v>mortality_level</v>
       </c>
-      <c r="L40" t="s">
-        <v>58</v>
-      </c>
-      <c r="M40" t="s">
-        <v>108</v>
-      </c>
-      <c r="N40" t="s">
-        <v>201</v>
-      </c>
-      <c r="O40" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G40" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="H40" t="str">
+        <f t="shared" si="1"/>
+        <v>006d2c</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>126</v>
       </c>
@@ -4587,20 +4628,15 @@
         <f t="shared" si="0"/>
         <v>mortality_vol</v>
       </c>
-      <c r="L41" t="s">
-        <v>59</v>
-      </c>
-      <c r="M41" t="s">
-        <v>109</v>
-      </c>
-      <c r="N41" t="s">
-        <v>202</v>
-      </c>
-      <c r="O41" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>229</v>
+      </c>
+      <c r="H41" t="str">
+        <f t="shared" si="1"/>
+        <v>006d2c</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>125</v>
       </c>
@@ -4611,116 +4647,91 @@
         <f t="shared" si="0"/>
         <v>mortality_calamity</v>
       </c>
-      <c r="L42" t="s">
-        <v>60</v>
-      </c>
-      <c r="M42" t="s">
-        <v>110</v>
-      </c>
-      <c r="N42" t="s">
-        <v>200</v>
-      </c>
-      <c r="O42" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G42" s="72" t="s">
+        <v>230</v>
+      </c>
+      <c r="H42" t="str">
+        <f t="shared" si="1"/>
+        <v>006d2c</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>123</v>
+        <v>231</v>
       </c>
       <c r="C43" t="s">
         <v>119</v>
       </c>
       <c r="E43" t="str">
         <f t="shared" si="0"/>
-        <v>uncertainty</v>
-      </c>
-      <c r="L43" t="s">
-        <v>61</v>
-      </c>
-      <c r="M43" t="s">
-        <v>111</v>
-      </c>
-      <c r="N43" t="s">
-        <v>203</v>
-      </c>
-      <c r="O43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+        <v>morb_uncertainty</v>
+      </c>
+      <c r="G43" s="75" t="s">
+        <v>237</v>
+      </c>
+      <c r="H43" t="str">
+        <f t="shared" si="1"/>
+        <v>045a8d</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>122</v>
+        <v>232</v>
       </c>
       <c r="C44" t="s">
         <v>119</v>
       </c>
       <c r="E44" t="str">
         <f t="shared" si="0"/>
-        <v>volatility</v>
-      </c>
-      <c r="L44" t="s">
-        <v>62</v>
-      </c>
-      <c r="M44" t="s">
-        <v>112</v>
-      </c>
-      <c r="N44" t="s">
-        <v>204</v>
-      </c>
-      <c r="O44" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+        <v>morb_volatility</v>
+      </c>
+      <c r="G44" t="s">
+        <v>238</v>
+      </c>
+      <c r="H44" t="str">
+        <f t="shared" si="1"/>
+        <v>045a8d</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>121</v>
+        <v>233</v>
       </c>
       <c r="C45" t="s">
         <v>119</v>
       </c>
       <c r="E45" t="str">
         <f t="shared" si="0"/>
-        <v>prior</v>
-      </c>
-      <c r="L45" t="s">
-        <v>207</v>
-      </c>
-      <c r="M45" t="s">
-        <v>219</v>
-      </c>
-      <c r="N45" t="s">
-        <v>196</v>
-      </c>
-      <c r="O45" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+        <v>morb_prior</v>
+      </c>
+      <c r="G45" t="s">
+        <v>239</v>
+      </c>
+      <c r="H45" t="str">
+        <f t="shared" si="1"/>
+        <v>045a8d</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>120</v>
+        <v>234</v>
       </c>
       <c r="C46" t="s">
         <v>119</v>
       </c>
       <c r="E46" t="str">
         <f t="shared" si="0"/>
-        <v>calamity</v>
-      </c>
-      <c r="L46" t="s">
-        <v>208</v>
-      </c>
-      <c r="M46" t="s">
-        <v>216</v>
-      </c>
-      <c r="N46" t="s">
-        <v>175</v>
-      </c>
-      <c r="O46" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+        <v>morb_calamity</v>
+      </c>
+      <c r="G46" s="82" t="s">
+        <v>240</v>
+      </c>
+      <c r="H46" t="str">
+        <f t="shared" si="1"/>
+        <v>045a8d</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>118</v>
       </c>
@@ -4731,20 +4742,15 @@
         <f t="shared" si="0"/>
         <v>penc_uncertaincy</v>
       </c>
-      <c r="L47" t="s">
-        <v>209</v>
-      </c>
-      <c r="M47" t="s">
-        <v>215</v>
-      </c>
-      <c r="N47" t="s">
-        <v>176</v>
-      </c>
-      <c r="O47" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G47" s="83" t="s">
+        <v>242</v>
+      </c>
+      <c r="H47" t="str">
+        <f t="shared" si="1"/>
+        <v>810f7c</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>117</v>
       </c>
@@ -4755,20 +4761,15 @@
         <f t="shared" si="0"/>
         <v>penc_vol</v>
       </c>
-      <c r="L48" t="s">
-        <v>210</v>
-      </c>
-      <c r="M48" t="s">
-        <v>217</v>
-      </c>
-      <c r="N48" t="s">
-        <v>177</v>
-      </c>
-      <c r="O48" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G48" t="s">
+        <v>243</v>
+      </c>
+      <c r="H48" t="str">
+        <f t="shared" si="1"/>
+        <v>810f7c</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>116</v>
       </c>
@@ -4779,20 +4780,15 @@
         <f t="shared" si="0"/>
         <v>penc_prior</v>
       </c>
-      <c r="L49" t="s">
-        <v>211</v>
-      </c>
-      <c r="M49" t="s">
-        <v>218</v>
-      </c>
-      <c r="N49" t="s">
-        <v>174</v>
-      </c>
-      <c r="O49" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G49" t="s">
+        <v>244</v>
+      </c>
+      <c r="H49" t="str">
+        <f t="shared" si="1"/>
+        <v>810f7c</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>115</v>
       </c>
@@ -4803,70 +4799,78 @@
         <f t="shared" si="0"/>
         <v>penc_cat</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G50" s="84" t="s">
+        <v>230</v>
+      </c>
+      <c r="H50" t="str">
+        <f t="shared" si="1"/>
+        <v>810f7c</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E51" t="s">
         <v>211</v>
       </c>
-      <c r="G51" s="1">
+      <c r="G51" s="1" t="str">
         <f>VLOOKUP(SUBSTITUTE(E51,"_other",""),$E$2:$G$50,3,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="H51">
+        <v>ffffff</v>
+      </c>
+      <c r="H51" t="str">
         <f>G51</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+        <v>ffffff</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E52" t="s">
         <v>220</v>
       </c>
-      <c r="G52" s="1">
+      <c r="F52" s="13"/>
+      <c r="G52" s="80" t="str">
         <f>VLOOKUP(SUBSTITUTE(E52,"_other",""),$E$2:$G$50,3,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="H52">
+        <v>990000</v>
+      </c>
+      <c r="H52" t="str">
         <f>G52</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+        <v>990000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E53" t="s">
         <v>209</v>
       </c>
-      <c r="G53" s="1">
+      <c r="G53" s="1" t="str">
         <f>VLOOKUP(SUBSTITUTE(E53,"_other",""),$E$2:$G$50,3,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="H53">
+        <v>006d2c</v>
+      </c>
+      <c r="H53" t="str">
         <f>G53</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+        <v>006d2c</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E54" t="s">
         <v>221</v>
       </c>
-      <c r="G54" s="1">
+      <c r="G54" s="1" t="str">
         <f>VLOOKUP(SUBSTITUTE(E54,"_other",""),$E$2:$G$50,3,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="H54">
+        <v>045a8d</v>
+      </c>
+      <c r="H54" t="str">
         <f>G54</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+        <v>045a8d</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E55" t="s">
         <v>222</v>
       </c>
-      <c r="G55" s="1">
+      <c r="G55" s="1" t="str">
         <f>VLOOKUP(SUBSTITUTE(E55,"_other",""),$E$2:$G$50,3,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="H55">
+        <v>810f7c</v>
+      </c>
+      <c r="H55" t="str">
         <f>G55</f>
-        <v>0</v>
+        <v>810f7c</v>
       </c>
     </row>
   </sheetData>
@@ -4881,7 +4885,9 @@
   </sheetPr>
   <dimension ref="A1:BA2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4925,152 +4931,153 @@
       <c r="D1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="L1" s="27" t="s">
-        <v>156</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="O1" s="27" t="s">
-        <v>152</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="R1" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="T1" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="U1" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="V1" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="W1" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="X1" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="Y1" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="Z1" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="AA1" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="AB1" s="23" t="s">
-        <v>141</v>
-      </c>
-      <c r="AC1" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="AD1" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="AE1" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="AF1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="AG1" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="AH1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="AI1" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="AJ1" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="AK1" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="AL1" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="AM1" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="AN1" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="AO1" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="AP1" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="AQ1" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="AR1" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="AS1" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="AT1" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="AU1" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="AV1" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="AW1" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="AX1" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="AY1" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="AZ1" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="BA1" s="7" t="s">
-        <v>115</v>
+      <c r="E1" s="23" t="str">
+        <f t="array" ref="E1:BA1">TRANSPOSE(ex6_struct_and_colors!A2:A50)</f>
+        <v>SCR</v>
+      </c>
+      <c r="F1" s="23" t="str">
+        <v>BSCR</v>
+      </c>
+      <c r="G1" s="7" t="str">
+        <v>operational</v>
+      </c>
+      <c r="H1" s="44" t="str">
+        <v>Adjustment-LACDT</v>
+      </c>
+      <c r="I1" s="27" t="str">
+        <v>BSCR_div</v>
+      </c>
+      <c r="J1" s="7" t="str">
+        <v>MBC</v>
+      </c>
+      <c r="K1" s="7" t="str">
+        <v>insurance</v>
+      </c>
+      <c r="L1" s="27" t="str">
+        <v>MBC_div</v>
+      </c>
+      <c r="M1" s="7" t="str">
+        <v>MC</v>
+      </c>
+      <c r="N1" s="7" t="str">
+        <v>basis</v>
+      </c>
+      <c r="O1" s="27" t="str">
+        <v>MC_div</v>
+      </c>
+      <c r="P1" s="7" t="str">
+        <v>market</v>
+      </c>
+      <c r="Q1" s="7" t="str">
+        <v>counterpartydefault</v>
+      </c>
+      <c r="R1" s="27" t="str">
+        <v>market_div</v>
+      </c>
+      <c r="S1" s="7" t="str">
+        <v>equity</v>
+      </c>
+      <c r="T1" s="7" t="str">
+        <v>interest</v>
+      </c>
+      <c r="U1" s="7" t="str">
+        <v>creditspread</v>
+      </c>
+      <c r="V1" s="7" t="str">
+        <v>realestate</v>
+      </c>
+      <c r="W1" s="7" t="str">
+        <v>inflation</v>
+      </c>
+      <c r="X1" s="7" t="str">
+        <v>equity_impliedvol</v>
+      </c>
+      <c r="Y1" s="7" t="str">
+        <v>interest_impliedvol</v>
+      </c>
+      <c r="Z1" s="7" t="str">
+        <v>FX</v>
+      </c>
+      <c r="AA1" s="7" t="str">
+        <v>FX_impliedvol</v>
+      </c>
+      <c r="AB1" s="23" t="str">
+        <v>type1</v>
+      </c>
+      <c r="AC1" s="7" t="str">
+        <v>type2</v>
+      </c>
+      <c r="AD1" s="27" t="str">
+        <v>insurance_div</v>
+      </c>
+      <c r="AE1" s="7" t="str">
+        <v>business</v>
+      </c>
+      <c r="AF1" s="7" t="str">
+        <v>life</v>
+      </c>
+      <c r="AG1" s="7" t="str">
+        <v>morbidity</v>
+      </c>
+      <c r="AH1" s="7" t="str">
+        <v>nonlife</v>
+      </c>
+      <c r="AI1" s="23" t="str">
+        <v>expense_level</v>
+      </c>
+      <c r="AJ1" s="7" t="str">
+        <v>expense_inflation</v>
+      </c>
+      <c r="AK1" s="7" t="str">
+        <v>continuation</v>
+      </c>
+      <c r="AL1" s="7" t="str">
+        <v>persistency_uncertain</v>
+      </c>
+      <c r="AM1" s="7" t="str">
+        <v>persistency_volatility</v>
+      </c>
+      <c r="AN1" s="7" t="str">
+        <v>persistency_calamity</v>
+      </c>
+      <c r="AO1" s="7" t="str">
+        <v>premium_rerating</v>
+      </c>
+      <c r="AP1" s="23" t="str">
+        <v>mortality_trend</v>
+      </c>
+      <c r="AQ1" s="7" t="str">
+        <v>mortality_level</v>
+      </c>
+      <c r="AR1" s="7" t="str">
+        <v>mortality_vol</v>
+      </c>
+      <c r="AS1" s="7" t="str">
+        <v>mortality_calamity</v>
+      </c>
+      <c r="AT1" s="23" t="str">
+        <v>morb_uncertainty</v>
+      </c>
+      <c r="AU1" s="7" t="str">
+        <v>morb_volatility</v>
+      </c>
+      <c r="AV1" s="7" t="str">
+        <v>morb_prior</v>
+      </c>
+      <c r="AW1" s="7" t="str">
+        <v>morb_calamity</v>
+      </c>
+      <c r="AX1" s="23" t="str">
+        <v>penc_uncertaincy</v>
+      </c>
+      <c r="AY1" s="7" t="str">
+        <v>penc_vol</v>
+      </c>
+      <c r="AZ1" s="7" t="str">
+        <v>penc_prior</v>
+      </c>
+      <c r="BA1" s="7" t="str">
+        <v>penc_cat</v>
       </c>
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.25">
@@ -5987,7 +5994,7 @@
   <dimension ref="A1:AU3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AN3" sqref="AN3"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6038,135 +6045,135 @@
       <c r="D1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="23" t="e">
-        <f t="array" ref="E1:AU1">TRANSPOSE(#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F1" s="26" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="G1" s="20" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="H1" s="29" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="I1" s="27" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="J1" s="20" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="K1" s="20" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="L1" s="20" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="M1" s="20" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="N1" s="20" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="O1" s="20" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="P1" s="27" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="Q1" s="20" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="R1" s="20" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="S1" s="20" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="T1" s="20" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="U1" s="20" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="V1" s="20" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="W1" s="20" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="X1" s="27" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="Y1" s="20" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="Z1" s="20" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AA1" s="20" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AB1" s="20" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AC1" s="20" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AD1" s="20" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AE1" s="20" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AF1" s="27" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AG1" s="20" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AH1" s="20" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AI1" s="20" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AJ1" s="27" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AK1" s="20" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AL1" s="20" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AM1" s="20" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AN1" s="20" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AO1" s="27" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AP1" s="7" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AQ1" s="7" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AR1" s="7" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AS1" s="7" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AT1" s="7" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AU1" s="7" t="e">
-        <v>#REF!</v>
+      <c r="E1" s="23" t="str">
+        <f t="array" ref="E1:AU1">TRANSPOSE(struct_and_colors_sf16!B2:B44)</f>
+        <v>SKV</v>
+      </c>
+      <c r="F1" s="26" t="str">
+        <v>KSKV</v>
+      </c>
+      <c r="G1" s="20" t="str">
+        <v>operationeel</v>
+      </c>
+      <c r="H1" s="29" t="str">
+        <v>LACDT</v>
+      </c>
+      <c r="I1" s="27" t="str">
+        <v>KSKV-div</v>
+      </c>
+      <c r="J1" s="20" t="str">
+        <v>markt</v>
+      </c>
+      <c r="K1" s="20" t="str">
+        <v>leven</v>
+      </c>
+      <c r="L1" s="20" t="str">
+        <v>schade</v>
+      </c>
+      <c r="M1" s="20" t="str">
+        <v>zorg</v>
+      </c>
+      <c r="N1" s="20" t="str">
+        <v>tegenpartijkrediet</v>
+      </c>
+      <c r="O1" s="20" t="str">
+        <v>intangibles</v>
+      </c>
+      <c r="P1" s="27" t="str">
+        <v>markt-div</v>
+      </c>
+      <c r="Q1" s="20" t="str">
+        <v>m_rente</v>
+      </c>
+      <c r="R1" s="20" t="str">
+        <v>m_aandelen</v>
+      </c>
+      <c r="S1" s="20" t="str">
+        <v>m_vastgoed</v>
+      </c>
+      <c r="T1" s="20" t="str">
+        <v>m_spread</v>
+      </c>
+      <c r="U1" s="20" t="str">
+        <v>m_valuta</v>
+      </c>
+      <c r="V1" s="20" t="str">
+        <v>m_concentratie</v>
+      </c>
+      <c r="W1" s="20" t="str">
+        <v>m_illiquiditeit</v>
+      </c>
+      <c r="X1" s="27" t="str">
+        <v>leven-div</v>
+      </c>
+      <c r="Y1" s="20" t="str">
+        <v>l_kortleven</v>
+      </c>
+      <c r="Z1" s="20" t="str">
+        <v>l_langleven</v>
+      </c>
+      <c r="AA1" s="20" t="str">
+        <v>l_ao</v>
+      </c>
+      <c r="AB1" s="20" t="str">
+        <v>l_verval</v>
+      </c>
+      <c r="AC1" s="20" t="str">
+        <v>l_kosten</v>
+      </c>
+      <c r="AD1" s="20" t="str">
+        <v>l_revisie</v>
+      </c>
+      <c r="AE1" s="20" t="str">
+        <v>l_CAT</v>
+      </c>
+      <c r="AF1" s="27" t="str">
+        <v>schade-div</v>
+      </c>
+      <c r="AG1" s="20" t="str">
+        <v>s_premiereserve</v>
+      </c>
+      <c r="AH1" s="20" t="str">
+        <v>s_verval</v>
+      </c>
+      <c r="AI1" s="20" t="str">
+        <v>s_CAT</v>
+      </c>
+      <c r="AJ1" s="27" t="str">
+        <v>zorg-div</v>
+      </c>
+      <c r="AK1" s="20" t="str">
+        <v>z_alsleven</v>
+      </c>
+      <c r="AL1" s="20" t="str">
+        <v>z_CAT</v>
+      </c>
+      <c r="AM1" s="20" t="str">
+        <v>z_s_premiereserve</v>
+      </c>
+      <c r="AN1" s="20" t="str">
+        <v>z_s_verval</v>
+      </c>
+      <c r="AO1" s="27" t="str">
+        <v>z_alsleven-div</v>
+      </c>
+      <c r="AP1" s="7" t="str">
+        <v>z_a_kortleven</v>
+      </c>
+      <c r="AQ1" s="7" t="str">
+        <v>z_a_langleven</v>
+      </c>
+      <c r="AR1" s="7" t="str">
+        <v>z_a_ao</v>
+      </c>
+      <c r="AS1" s="7" t="str">
+        <v>z_a_verval</v>
+      </c>
+      <c r="AT1" s="7" t="str">
+        <v>z_a_kosten</v>
+      </c>
+      <c r="AU1" s="7" t="str">
+        <v>z_a_revisie</v>
       </c>
     </row>
     <row r="2" spans="1:47" x14ac:dyDescent="0.25">
@@ -7787,7 +7794,7 @@
   <dimension ref="A1:AU5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+      <selection activeCell="AO12" sqref="AO12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7843,135 +7850,135 @@
       <c r="D1" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="55" t="e">
-        <f t="array" ref="E1:AU1">TRANSPOSE(#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F1" s="56" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="G1" s="57" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="H1" s="58" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="I1" s="59" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="J1" s="57" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="K1" s="57" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="L1" s="57" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="M1" s="57" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="N1" s="57" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="O1" s="57" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="P1" s="59" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="Q1" s="57" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="R1" s="57" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="S1" s="57" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="T1" s="57" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="U1" s="57" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="V1" s="57" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="W1" s="57" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="X1" s="59" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="Y1" s="57" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="Z1" s="57" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AA1" s="57" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AB1" s="57" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AC1" s="57" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AD1" s="57" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AE1" s="57" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AF1" s="59" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AG1" s="57" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AH1" s="57" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AI1" s="57" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AJ1" s="59" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AK1" s="57" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AL1" s="57" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AM1" s="57" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AN1" s="57" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AO1" s="59" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AP1" s="60" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AQ1" s="60" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AR1" s="60" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AS1" s="60" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AT1" s="60" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AU1" s="60" t="e">
-        <v>#REF!</v>
+      <c r="E1" s="55" t="str">
+        <f t="array" ref="E1:AU1">TRANSPOSE(struct_and_colors_sf16!A2:A44)</f>
+        <v>SCR</v>
+      </c>
+      <c r="F1" s="56" t="str">
+        <v>BSCR</v>
+      </c>
+      <c r="G1" s="57" t="str">
+        <v>operational</v>
+      </c>
+      <c r="H1" s="58" t="str">
+        <v>Adjustment-LACDT</v>
+      </c>
+      <c r="I1" s="59" t="str">
+        <v>BSCR_div</v>
+      </c>
+      <c r="J1" s="57" t="str">
+        <v>market</v>
+      </c>
+      <c r="K1" s="57" t="str">
+        <v>life</v>
+      </c>
+      <c r="L1" s="57" t="str">
+        <v>non-life</v>
+      </c>
+      <c r="M1" s="57" t="str">
+        <v>health</v>
+      </c>
+      <c r="N1" s="57" t="str">
+        <v>cp-default</v>
+      </c>
+      <c r="O1" s="57" t="str">
+        <v>intangibles</v>
+      </c>
+      <c r="P1" s="59" t="str">
+        <v>market_div</v>
+      </c>
+      <c r="Q1" s="57" t="str">
+        <v>m_interestrate</v>
+      </c>
+      <c r="R1" s="57" t="str">
+        <v>m_equity</v>
+      </c>
+      <c r="S1" s="57" t="str">
+        <v>m_property</v>
+      </c>
+      <c r="T1" s="57" t="str">
+        <v>m_spread</v>
+      </c>
+      <c r="U1" s="57" t="str">
+        <v>m_currency</v>
+      </c>
+      <c r="V1" s="57" t="str">
+        <v>m_concentration</v>
+      </c>
+      <c r="W1" s="57" t="str">
+        <v>m_illiquidity</v>
+      </c>
+      <c r="X1" s="59" t="str">
+        <v>life_div</v>
+      </c>
+      <c r="Y1" s="57" t="str">
+        <v>l_mortality</v>
+      </c>
+      <c r="Z1" s="57" t="str">
+        <v>l_longevity</v>
+      </c>
+      <c r="AA1" s="57" t="str">
+        <v>l_disability</v>
+      </c>
+      <c r="AB1" s="57" t="str">
+        <v>l_lapse</v>
+      </c>
+      <c r="AC1" s="57" t="str">
+        <v>l_expenses</v>
+      </c>
+      <c r="AD1" s="57" t="str">
+        <v>l_revision</v>
+      </c>
+      <c r="AE1" s="57" t="str">
+        <v>l_CAT</v>
+      </c>
+      <c r="AF1" s="59" t="str">
+        <v>nonlife_div</v>
+      </c>
+      <c r="AG1" s="57" t="str">
+        <v>n_premiumreserve</v>
+      </c>
+      <c r="AH1" s="57" t="str">
+        <v>n_lapse</v>
+      </c>
+      <c r="AI1" s="57" t="str">
+        <v>n_CAT</v>
+      </c>
+      <c r="AJ1" s="59" t="str">
+        <v>health_div</v>
+      </c>
+      <c r="AK1" s="57" t="str">
+        <v>h_SLT</v>
+      </c>
+      <c r="AL1" s="57" t="str">
+        <v>h_CAT</v>
+      </c>
+      <c r="AM1" s="57" t="str">
+        <v>h_n_premiumres</v>
+      </c>
+      <c r="AN1" s="57" t="str">
+        <v>h_n_lapse</v>
+      </c>
+      <c r="AO1" s="59" t="str">
+        <v>h_SLT_div</v>
+      </c>
+      <c r="AP1" s="60" t="str">
+        <v>h_s_mortality</v>
+      </c>
+      <c r="AQ1" s="60" t="str">
+        <v>h_s_longevity</v>
+      </c>
+      <c r="AR1" s="60" t="str">
+        <v>h_s_disability</v>
+      </c>
+      <c r="AS1" s="60" t="str">
+        <v>h_s_lapse</v>
+      </c>
+      <c r="AT1" s="60" t="str">
+        <v>h_s_expenses</v>
+      </c>
+      <c r="AU1" s="60" t="str">
+        <v>h_s_revision</v>
       </c>
     </row>
     <row r="2" spans="1:47" x14ac:dyDescent="0.25">
@@ -8500,7 +8507,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8775,8 +8782,8 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>5</v>
+      <c r="A19" s="13" t="s">
+        <v>223</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
@@ -9072,8 +9079,8 @@
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9169,7 +9176,7 @@
         <v>33.564</v>
       </c>
       <c r="L2" s="14">
-        <v>0.48399999999999999</v>
+        <v>5</v>
       </c>
       <c r="M2" s="19">
         <v>1</v>
@@ -9210,7 +9217,7 @@
         <v>40.002000000000002</v>
       </c>
       <c r="L3" s="9">
-        <v>1.23</v>
+        <v>7</v>
       </c>
       <c r="M3" s="18"/>
     </row>
@@ -9249,7 +9256,7 @@
         <v>28.87</v>
       </c>
       <c r="L4" s="9">
-        <v>0.49</v>
+        <v>8</v>
       </c>
       <c r="M4" s="18">
         <v>2</v>

</xml_diff>